<commit_message>
chosen motor & driver HW, updated documentation
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -662,9 +662,6 @@
     <t>how to implement DC motor:</t>
   </si>
   <si>
-    <t>Size H x W x L</t>
-  </si>
-  <si>
     <t>mN*m</t>
   </si>
   <si>
@@ -970,6 +967,63 @@
   <si>
     <t>Wire color</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Final solution:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Driver</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+POLOLU 2135
+http://www.tme.eu/ro/details/pololu-2135/drivere-modulare-de-motor/pololu/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Motor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+POLOLU 2368 - MP - 150:1
+http://www.tme.eu/ro/details/pololu-2368/micromotoare-si-accesorii/pololu/150_1-micro-metal-gearmotor-mp/
+https://www.pololu.com/product/2368
+https://www.pololu.com/product/2368/resources</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -978,7 +1032,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1141,6 +1195,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1559,7 +1629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1671,6 +1741,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1680,11 +1755,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4988,10 +5061,10 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="62"/>
       <c r="B2" s="61" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="61" t="s">
         <v>183</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -5000,247 +5073,247 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
       <c r="B5" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>
       <c r="B7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="62"/>
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="62"/>
       <c r="B9" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
       <c r="B10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="62"/>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="62"/>
       <c r="B12" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E12" s="59"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="62"/>
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C13" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
       <c r="B14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="62"/>
       <c r="B15" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="62"/>
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="62"/>
       <c r="B17" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C17" s="46"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
       <c r="B18" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="62"/>
       <c r="B19" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="62"/>
       <c r="B20" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="62"/>
       <c r="B21" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="62"/>
       <c r="B22" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="62"/>
       <c r="B23" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="62"/>
       <c r="B24" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="62"/>
       <c r="B25" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="62" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C27" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" t="s">
         <v>238</v>
-      </c>
-      <c r="D27" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5249,72 +5322,72 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="62"/>
       <c r="B29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>167</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="62"/>
       <c r="B30" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="62"/>
       <c r="B35" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -5326,10 +5399,10 @@
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="62"/>
       <c r="B38" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -5337,31 +5410,31 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="46" t="s">
         <v>177</v>
-      </c>
-      <c r="C40" s="46" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="62"/>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" s="60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="62"/>
       <c r="B42" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6812,35 +6885,35 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L2" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="M2" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="M2" s="70" t="s">
+      <c r="N2" s="70" t="s">
         <v>216</v>
-      </c>
-      <c r="N2" s="70" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6848,24 +6921,24 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" t="s">
         <v>220</v>
-      </c>
-      <c r="N5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -6873,10 +6946,10 @@
         <v>3</v>
       </c>
       <c r="M6" t="s">
+        <v>221</v>
+      </c>
+      <c r="N6" t="s">
         <v>222</v>
-      </c>
-      <c r="N6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -6909,7 +6982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -6937,18 +7010,18 @@
       <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="83" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="84" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -6957,24 +7030,24 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="82"/>
+      <c r="F2" s="79"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="82"/>
+      <c r="F3" s="79"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
+      <c r="A4" s="84"/>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
@@ -6987,16 +7060,16 @@
       <c r="E4" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="79" t="s">
         <v>59</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>174</v>
-      </c>
-      <c r="H4" s="84"/>
+        <v>173</v>
+      </c>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="84"/>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
@@ -7009,30 +7082,30 @@
       <c r="E5" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="79" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="83" t="s">
+      <c r="F6" s="80" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
@@ -7045,16 +7118,16 @@
       <c r="E7" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="82" t="s">
+      <c r="F7" s="79" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" s="85"/>
+        <v>171</v>
+      </c>
+      <c r="H7" s="82"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="1" t="s">
         <v>47</v>
       </c>
@@ -7067,16 +7140,16 @@
       <c r="E8" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="79" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H8" s="58"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
@@ -7089,16 +7162,16 @@
       <c r="E9" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="F9" s="79" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="84" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -7113,14 +7186,14 @@
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="82" t="s">
+      <c r="F11" s="79" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -7133,14 +7206,14 @@
       <c r="E12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="82" t="s">
+      <c r="F12" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="84" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -7150,19 +7223,19 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="82" t="s">
+      <c r="F14" s="79" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -7170,19 +7243,19 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="79" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="84" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -7197,14 +7270,14 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="82" t="s">
+      <c r="F17" s="79" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -7212,19 +7285,19 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="79" t="s">
         <v>151</v>
-      </c>
-      <c r="F18" s="82" t="s">
-        <v>152</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
+      <c r="A19" s="84"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
@@ -7232,19 +7305,19 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="82" t="s">
+      <c r="F19" s="79" t="s">
         <v>31</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
@@ -7252,19 +7325,19 @@
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="82" t="s">
+      <c r="F20" s="79" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -7277,7 +7350,7 @@
       <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="82" t="s">
+      <c r="F21" s="79" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="1"/>
@@ -7305,57 +7378,57 @@
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="76" t="s">
+        <v>224</v>
+      </c>
+      <c r="C28" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="C28" s="77" t="s">
-        <v>226</v>
-      </c>
       <c r="D28" s="78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D29" s="72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D30" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="73" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C32" s="74" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -7383,17 +7456,17 @@
   <sheetData>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -7595,7 +7668,7 @@
         <v>13333332.000000002</v>
       </c>
       <c r="D6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6">
         <f>E7*1000/E8</f>
@@ -7612,7 +7685,7 @@
       </c>
       <c r="C7" s="68"/>
       <c r="D7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7">
         <v>5000</v>
@@ -7621,7 +7694,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E8">
         <v>16000</v>
@@ -7683,7 +7756,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -7694,10 +7767,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7709,7 +7782,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
@@ -7729,7 +7802,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>112</v>
       </c>
@@ -7752,11 +7825,8 @@
       <c r="G2" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I2" t="s">
-        <v>140</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>114</v>
       </c>
@@ -7784,15 +7854,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="85" t="s">
         <v>115</v>
       </c>
       <c r="B5" s="47">
@@ -7813,9 +7883,19 @@
       <c r="G5" s="46" t="s">
         <v>116</v>
       </c>
+      <c r="I5" s="87" t="s">
+        <v>242</v>
+      </c>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="80"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="85"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -7839,16 +7919,32 @@
       <c r="G6" s="46" t="s">
         <v>117</v>
       </c>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="86" t="s">
         <v>118</v>
       </c>
       <c r="B8" s="50">
@@ -7874,9 +7970,17 @@
       <c r="G8" s="46" t="s">
         <v>119</v>
       </c>
+      <c r="I8" s="87"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="81"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="86"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -7900,9 +8004,17 @@
       <c r="G9" s="46" t="s">
         <v>120</v>
       </c>
+      <c r="I9" s="87"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="81"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="86"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -7926,9 +8038,17 @@
       <c r="G10" s="46" t="s">
         <v>121</v>
       </c>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="87"/>
+      <c r="P10" s="87"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="81"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="86"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -7952,16 +8072,32 @@
       <c r="G11" s="46" t="s">
         <v>122</v>
       </c>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="80" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="85" t="s">
         <v>123</v>
       </c>
       <c r="B13" s="47">
@@ -7982,9 +8118,17 @@
       <c r="G13" s="46" t="s">
         <v>124</v>
       </c>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="87"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="80"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="85"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -8008,9 +8152,17 @@
       <c r="G14" s="46" t="s">
         <v>125</v>
       </c>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="87"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="85"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -8032,11 +8184,19 @@
         <v>49.430864</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>141</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="80"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="85"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -8060,9 +8220,17 @@
       <c r="G16" s="46" t="s">
         <v>126</v>
       </c>
+      <c r="I16" s="87"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="87"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="80" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="85" t="s">
         <v>127</v>
       </c>
       <c r="B17" s="50">
@@ -8088,9 +8256,17 @@
       <c r="G17" s="46" t="s">
         <v>128</v>
       </c>
+      <c r="I17" s="87"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="85"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -8114,8 +8290,16 @@
       <c r="G18" s="46" t="s">
         <v>129</v>
       </c>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>130</v>
       </c>
@@ -8132,22 +8316,22 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -8155,17 +8339,18 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A17:A18"/>
+    <mergeCell ref="I5:P18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B24" r:id="rId1"/>
@@ -16392,7 +16577,7 @@
       <c r="CE1" s="7"/>
       <c r="CF1" s="8"/>
       <c r="CH1" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="CW1" s="6"/>
       <c r="CX1" s="7"/>
@@ -21052,7 +21237,7 @@
       <c r="AN25" s="11"/>
       <c r="AO25" s="11"/>
       <c r="AP25" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AQ25" s="11"/>
       <c r="AR25" s="11"/>

</xml_diff>

<commit_message>
Started developing CAN init function
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Wellcome IMG WIP" sheetId="6" r:id="rId9"/>
     <sheet name="Font and symbol Hex Gen" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="264">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Output</t>
-  </si>
-  <si>
-    <t>Level Interrupt</t>
   </si>
   <si>
     <t>PF2 ( Blue LED)</t>
@@ -1042,15 +1039,63 @@
   <si>
     <t>Toggle PF2 and PF3 with PWM on / off, commanded by 2nd uC through CAN</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>PB4</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>PE4</t>
+  </si>
+  <si>
+    <t>PE5</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>GPIO for SPI / SSI</t>
+  </si>
+  <si>
+    <t>GPIO for Level Interrupt</t>
+  </si>
+  <si>
+    <t>PE0</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PE2</t>
+  </si>
+  <si>
+    <t>PE3</t>
+  </si>
+  <si>
+    <t>CAN0Rx</t>
+  </si>
+  <si>
+    <t>CAN0Tx</t>
+  </si>
+  <si>
+    <t>CAN module 0 transmit.</t>
+  </si>
+  <si>
+    <t>CAN module 0 receive.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2383,13 +2428,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>3295650</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2403,7 +2448,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2423,7 +2468,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -4801,7 +4846,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4833,10 +4878,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4868,7 +4912,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5044,21 +5087,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -5076,465 +5119,465 @@
       <c r="O1" s="62"/>
       <c r="P1" s="62"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="62"/>
       <c r="B2" s="61" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="61" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="61" t="s">
-        <v>181</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="62"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="62"/>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="62"/>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="62"/>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="62"/>
       <c r="B7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="62"/>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="62"/>
       <c r="B9" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="62"/>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="62"/>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="62"/>
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C12" s="58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="62"/>
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="58" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="62"/>
       <c r="B14" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="58" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="62"/>
       <c r="B15" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="58" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="62"/>
       <c r="B16" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="62"/>
       <c r="B17" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="62"/>
       <c r="B18" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="62"/>
       <c r="B19" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="62"/>
       <c r="B20" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="62"/>
       <c r="B21" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="62"/>
       <c r="B22" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="62"/>
       <c r="B23" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="62"/>
       <c r="B24" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="62" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="60" t="s">
         <v>233</v>
       </c>
+      <c r="D26" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C26" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="D26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="62"/>
       <c r="B27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="62"/>
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="62"/>
       <c r="B29" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="62"/>
       <c r="B30" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="62"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="62"/>
       <c r="B32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="C32" s="46" t="s">
-        <v>165</v>
-      </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="62"/>
       <c r="B33" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>243</v>
+    <row r="37" spans="1:3">
+      <c r="A37" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="62" t="s">
-        <v>237</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="62"/>
       <c r="B38" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="62"/>
       <c r="B39" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="62"/>
       <c r="B41" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="62"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="46" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="46" t="s">
-        <v>175</v>
-      </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="62"/>
       <c r="B44" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C44" s="60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="62"/>
       <c r="B45" s="46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45" s="58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="62"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="62"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="62"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="62"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="62"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="62"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="62"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="62"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="62"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="62"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="62"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="62"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="62"/>
     </row>
   </sheetData>
@@ -5544,14 +5587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="63" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="63" customWidth="1"/>
@@ -5567,7 +5610,7 @@
     <col min="40" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39">
       <c r="A1" s="65"/>
       <c r="B1" s="65"/>
       <c r="C1" s="66"/>
@@ -5604,7 +5647,7 @@
       <c r="AL1" s="66"/>
       <c r="AM1" s="66"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39">
       <c r="A2" s="65"/>
       <c r="B2" s="67"/>
       <c r="C2" s="67">
@@ -5653,7 +5696,7 @@
       <c r="AL2" s="67"/>
       <c r="AM2" s="66"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39">
       <c r="A3" s="65"/>
       <c r="B3" s="67">
         <v>1</v>
@@ -5712,7 +5755,7 @@
       <c r="AL3" s="67"/>
       <c r="AM3" s="66"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39">
       <c r="A4" s="65"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67">
@@ -5773,7 +5816,7 @@
       <c r="AL4" s="67"/>
       <c r="AM4" s="66"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39">
       <c r="A5" s="65"/>
       <c r="B5" s="67">
         <v>1</v>
@@ -5838,7 +5881,7 @@
       </c>
       <c r="AM5" s="66"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39">
       <c r="A6" s="65"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67">
@@ -5903,7 +5946,7 @@
       </c>
       <c r="AM6" s="66"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39">
       <c r="A7" s="65"/>
       <c r="B7" s="67">
         <v>1</v>
@@ -5970,7 +6013,7 @@
       <c r="AL7" s="67"/>
       <c r="AM7" s="66"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39">
       <c r="A8" s="65"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67">
@@ -6031,7 +6074,7 @@
       <c r="AL8" s="67"/>
       <c r="AM8" s="65"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39">
       <c r="A9" s="65"/>
       <c r="B9" s="67">
         <v>1</v>
@@ -6092,7 +6135,7 @@
       <c r="AL9" s="67"/>
       <c r="AM9" s="65"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39">
       <c r="A10" s="65"/>
       <c r="B10" s="65"/>
       <c r="C10" s="65"/>
@@ -6129,7 +6172,7 @@
       <c r="AL10" s="65"/>
       <c r="AM10" s="65"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39">
       <c r="B12" s="64" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -6231,7 +6274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39">
       <c r="A14" s="65"/>
       <c r="B14" s="65"/>
       <c r="C14" s="66"/>
@@ -6268,7 +6311,7 @@
       <c r="AL14" s="66"/>
       <c r="AM14" s="66"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39">
       <c r="A15" s="65"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -6311,7 +6354,7 @@
       <c r="AL15" s="67"/>
       <c r="AM15" s="66"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39">
       <c r="A16" s="65"/>
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
@@ -6364,7 +6407,7 @@
       <c r="AL16" s="67"/>
       <c r="AM16" s="66"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39">
       <c r="A17" s="65"/>
       <c r="B17" s="67">
         <v>1</v>
@@ -6437,7 +6480,7 @@
       </c>
       <c r="AM17" s="66"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39">
       <c r="A18" s="65"/>
       <c r="B18" s="67"/>
       <c r="C18" s="67">
@@ -6500,7 +6543,7 @@
       </c>
       <c r="AM18" s="66"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39">
       <c r="A19" s="65"/>
       <c r="B19" s="67"/>
       <c r="C19" s="67"/>
@@ -6551,7 +6594,7 @@
       </c>
       <c r="AM19" s="66"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39">
       <c r="A20" s="65"/>
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
@@ -6604,7 +6647,7 @@
       </c>
       <c r="AM20" s="66"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39">
       <c r="A21" s="65"/>
       <c r="B21" s="67"/>
       <c r="C21" s="67">
@@ -6663,7 +6706,7 @@
       <c r="AL21" s="67"/>
       <c r="AM21" s="65"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39">
       <c r="A22" s="65"/>
       <c r="B22" s="67"/>
       <c r="C22" s="67"/>
@@ -6706,7 +6749,7 @@
       <c r="AL22" s="67"/>
       <c r="AM22" s="65"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39">
       <c r="A23" s="65"/>
       <c r="B23" s="65"/>
       <c r="C23" s="65"/>
@@ -6743,7 +6786,7 @@
       <c r="AL23" s="65"/>
       <c r="AM23" s="65"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39">
       <c r="B25" s="64" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -6931,104 +6974,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="69" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L1" s="69" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" s="70" t="s">
         <v>210</v>
       </c>
+      <c r="M2" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="N2" s="70" t="s">
+        <v>212</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
         <v>197</v>
-      </c>
-      <c r="L2" s="70" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="70" t="s">
-        <v>212</v>
-      </c>
-      <c r="N2" s="70" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>198</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5" t="s">
+        <v>215</v>
+      </c>
+      <c r="N5" t="s">
         <v>216</v>
       </c>
-      <c r="N5" t="s">
-        <v>217</v>
-      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="L6">
         <v>3</v>
       </c>
       <c r="M6" t="s">
+        <v>217</v>
+      </c>
+      <c r="N6" t="s">
         <v>218</v>
       </c>
-      <c r="N6" t="s">
-        <v>219</v>
-      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="L7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="L8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="L9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="L10">
         <v>7</v>
       </c>
@@ -7040,25 +7083,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -7069,24 +7112,24 @@
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" s="83" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="84" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7095,10 +7138,10 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="84"/>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -7107,397 +7150,511 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="84"/>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H4" s="81"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="84"/>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="84"/>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="80" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="84"/>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H7" s="82"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="84"/>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>254</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="79" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H8" s="58"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="84"/>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E9" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="60" t="s">
-        <v>50</v>
-      </c>
       <c r="F9" s="79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="84" t="s">
-        <v>34</v>
+        <v>248</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="79" t="s">
-        <v>5</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="84"/>
       <c r="B12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="79" t="s">
-        <v>39</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="84" t="s">
-        <v>32</v>
+        <v>253</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="79" t="s">
-        <v>25</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="84"/>
       <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="79" t="s">
-        <v>25</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="84" t="s">
-        <v>33</v>
-      </c>
+    <row r="16" spans="1:8">
+      <c r="A16" s="84"/>
+      <c r="B16" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="84"/>
       <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="79" t="s">
-        <v>15</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="84"/>
-      <c r="B18" s="2" t="s">
-        <v>13</v>
+      <c r="B18" s="1" t="s">
+        <v>251</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F18" s="79" t="s">
-        <v>151</v>
+        <v>260</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="84"/>
-      <c r="B19" s="3" t="s">
-        <v>11</v>
+      <c r="B19" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="79" t="s">
-        <v>31</v>
+        <v>261</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="79" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
+    <row r="21" spans="1:8">
+      <c r="A21" s="84" t="s">
+        <v>33</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="79" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="84"/>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="84"/>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="79" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1">
+      <c r="A27" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="79" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="A28" s="84"/>
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="84"/>
+      <c r="B29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="84"/>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="84"/>
+      <c r="B31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="C34" t="s">
         <v>19</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" thickBot="1"/>
+    <row r="38" spans="2:4">
+      <c r="B38" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" s="78" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D39" s="72" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="71" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" s="72" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D41" s="72" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="76" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="77" t="s">
-        <v>222</v>
-      </c>
-      <c r="D28" s="78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="71" t="s">
-        <v>223</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="71" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D30" s="72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="71" t="s">
+    <row r="42" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B42" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C42" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D42" s="75" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="C32" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="75" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A17:A21"/>
+  <mergeCells count="6">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A2:A9"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7506,28 +7663,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A13:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -7537,14 +7694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -7556,189 +7713,189 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="39">
         <v>1</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="44">
         <f>B1*10^3</f>
         <v>1000</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F1" s="43">
         <f>D1*10^3</f>
         <v>1000000</v>
       </c>
       <c r="G1" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H1" s="42">
         <f>D1*10^6</f>
         <v>1000000000</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="45">
         <f>1/B1</f>
         <v>1</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="44">
         <f>B2/10^3</f>
         <v>1E-3</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="43">
         <f>B2/10^6</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="42">
         <f>F2/10^3</f>
         <v>9.9999999999999986E-10</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="41">
         <f>(F3*10^6)</f>
         <v>13333333</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="40">
         <f>B3/10^3</f>
         <v>13333.333000000001</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="39">
         <f>13333333/1000000</f>
         <v>13.333333</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" s="37">
         <f>F3/10^3</f>
         <v>1.3333332999999999E-2</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="35">
         <f>1/B3</f>
         <v>7.5000001875000043E-8</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="34">
         <f>B4*10^3</f>
         <v>7.500000187500004E-5</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="33">
         <f>D4*10^3</f>
         <v>7.5000001875000041E-2</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="32">
         <f>B4*10^9</f>
         <v>75.000001875000038</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="29">
         <f>(H1/H4)-1</f>
         <v>13333332.000000002</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6">
         <f>E7*1000/E8</f>
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="29" t="str">
         <f>DEC2HEX(B6)</f>
@@ -7746,37 +7903,37 @@
       </c>
       <c r="C7" s="68"/>
       <c r="D7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E7">
         <v>5000</v>
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="D8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -7791,13 +7948,13 @@
         <v>319</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -7809,15 +7966,15 @@
         <v>639</v>
       </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="E20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -7827,14 +7984,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -7843,29 +8000,29 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="46" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>112</v>
       </c>
       <c r="B2" s="47">
         <v>42</v>
@@ -7884,12 +8041,12 @@
         <v>42</v>
       </c>
       <c r="G2" s="46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="46" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>114</v>
       </c>
       <c r="B3" s="50">
         <f>PI()*B2</f>
@@ -7912,19 +8069,19 @@
         <v>131.94689145077132</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
       <c r="A5" s="85" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="47">
         <v>50</v>
@@ -7942,10 +8099,10 @@
         <v>250</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J5" s="87"/>
       <c r="K5" s="87"/>
@@ -7955,7 +8112,7 @@
       <c r="O5" s="87"/>
       <c r="P5" s="87"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="85"/>
       <c r="B6" s="50">
         <f>B5/60</f>
@@ -7978,7 +8135,7 @@
         <v>4.166666666666667</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I6" s="87"/>
       <c r="J6" s="87"/>
@@ -7989,7 +8146,7 @@
       <c r="O6" s="87"/>
       <c r="P6" s="87"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -8004,9 +8161,9 @@
       <c r="O7" s="87"/>
       <c r="P7" s="87"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="50">
         <f>B3*B6</f>
@@ -8029,7 +8186,7 @@
         <v>549.77871437821386</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" s="87"/>
       <c r="J8" s="87"/>
@@ -8040,7 +8197,7 @@
       <c r="O8" s="87"/>
       <c r="P8" s="87"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="86"/>
       <c r="B9" s="50">
         <f>B8/10</f>
@@ -8063,7 +8220,7 @@
         <v>54.977871437821385</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I9" s="87"/>
       <c r="J9" s="87"/>
@@ -8074,7 +8231,7 @@
       <c r="O9" s="87"/>
       <c r="P9" s="87"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="86"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
@@ -8097,7 +8254,7 @@
         <v>0.54977871437821391</v>
       </c>
       <c r="G10" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I10" s="87"/>
       <c r="J10" s="87"/>
@@ -8108,7 +8265,7 @@
       <c r="O10" s="87"/>
       <c r="P10" s="87"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="86"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
@@ -8131,7 +8288,7 @@
         <v>1.97920337176157</v>
       </c>
       <c r="G11" s="46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I11" s="87"/>
       <c r="J11" s="87"/>
@@ -8142,7 +8299,7 @@
       <c r="O11" s="87"/>
       <c r="P11" s="87"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
@@ -8157,9 +8314,9 @@
       <c r="O12" s="87"/>
       <c r="P12" s="87"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B13" s="47">
         <v>32</v>
@@ -8177,7 +8334,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I13" s="87"/>
       <c r="J13" s="87"/>
@@ -8188,7 +8345,7 @@
       <c r="O13" s="87"/>
       <c r="P13" s="87"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="85"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
@@ -8211,7 +8368,7 @@
         <v>4.9430863999999998E-2</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I14" s="87"/>
       <c r="J14" s="87"/>
@@ -8222,7 +8379,7 @@
       <c r="O14" s="87"/>
       <c r="P14" s="87"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="85"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
@@ -8245,7 +8402,7 @@
         <v>49.430864</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I15" s="87"/>
       <c r="J15" s="87"/>
@@ -8256,7 +8413,7 @@
       <c r="O15" s="87"/>
       <c r="P15" s="87"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="85"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
@@ -8279,7 +8436,7 @@
         <v>49.430864</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I16" s="87"/>
       <c r="J16" s="87"/>
@@ -8290,9 +8447,9 @@
       <c r="O16" s="87"/>
       <c r="P16" s="87"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="50">
         <f>B16/(B2/2)</f>
@@ -8315,7 +8472,7 @@
         <v>2.3538506666666668</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I17" s="87"/>
       <c r="J17" s="87"/>
@@ -8326,7 +8483,7 @@
       <c r="O17" s="87"/>
       <c r="P17" s="87"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="85"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
@@ -8349,7 +8506,7 @@
         <v>0.23994400271831465</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I18" s="87"/>
       <c r="J18" s="87"/>
@@ -8360,49 +8517,49 @@
       <c r="O18" s="87"/>
       <c r="P18" s="87"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>131</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>132</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>133</v>
       </c>
-      <c r="F19" t="s">
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="54" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="54" t="s">
+    <row r="21" spans="1:16">
+      <c r="A21" s="55" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+    <row r="22" spans="1:16">
+      <c r="A22" s="56" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="57" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="57" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="B25" s="57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -8423,14 +8580,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="F2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -8498,7 +8655,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -8537,21 +8694,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
       <c r="A2" s="19">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20">
@@ -8561,34 +8718,34 @@
         <v>0</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="20"/>
       <c r="K2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="20" t="s">
-        <v>72</v>
-      </c>
       <c r="M2" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="48" customHeight="1">
       <c r="A3" s="19">
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>68</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20">
@@ -8598,7 +8755,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="20">
@@ -8611,25 +8768,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="48" customHeight="1">
       <c r="A4" s="19">
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -8638,18 +8795,18 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="48" customHeight="1">
       <c r="A5" s="19">
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="20">
@@ -8662,19 +8819,19 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="48" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="23" t="s">
         <v>77</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>78</v>
       </c>
       <c r="F6" s="20"/>
       <c r="H6" s="20"/>
@@ -8684,21 +8841,21 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
       <c r="A7" s="19">
         <v>5</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24">
@@ -8708,7 +8865,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" s="24">
         <v>5</v>
@@ -8719,21 +8876,21 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -8801,7 +8958,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -8887,10 +9044,10 @@
       <c r="CE1" s="7"/>
       <c r="CF1" s="8"/>
       <c r="CH1" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8980,7 +9137,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -9070,7 +9227,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -9194,7 +9351,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -9320,7 +9477,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -9438,7 +9595,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -9552,7 +9709,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -9664,7 +9821,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -9778,7 +9935,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -9890,7 +10047,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -10004,7 +10161,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -10164,7 +10321,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -10330,7 +10487,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -10494,7 +10651,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -10648,7 +10805,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -10802,7 +10959,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -10966,7 +11123,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -11134,7 +11291,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -11304,7 +11461,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -11456,7 +11613,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -11586,7 +11743,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -11702,7 +11859,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -11826,7 +11983,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -11950,7 +12107,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -12072,7 +12229,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -12192,7 +12349,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -12310,7 +12467,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -12424,7 +12581,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -12538,7 +12695,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -12648,7 +12805,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -12758,7 +12915,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -12868,7 +13025,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -12978,7 +13135,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -13088,7 +13245,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -13200,7 +13357,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -13314,7 +13471,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -13424,7 +13581,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -13534,7 +13691,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -13638,10 +13795,10 @@
       <c r="CE39" s="11"/>
       <c r="CF39" s="12"/>
       <c r="CH39" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -13739,7 +13896,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -13825,10 +13982,10 @@
       <c r="CE41" s="11"/>
       <c r="CF41" s="12"/>
       <c r="CH41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -13914,10 +14071,10 @@
       <c r="CE42" s="11"/>
       <c r="CF42" s="12"/>
       <c r="CH42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -14003,10 +14160,10 @@
       <c r="CE43" s="11"/>
       <c r="CF43" s="12"/>
       <c r="CH43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -14092,7 +14249,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -14178,7 +14335,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -14264,7 +14421,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -14350,7 +14507,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -14436,7 +14593,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -14774,7 +14931,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -15112,7 +15269,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -15450,7 +15607,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -15788,7 +15945,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -16126,7 +16283,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -16476,14 +16633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -16552,7 +16709,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -16638,7 +16795,7 @@
       <c r="CE1" s="7"/>
       <c r="CF1" s="8"/>
       <c r="CH1" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="CW1" s="6"/>
       <c r="CX1" s="7"/>
@@ -16725,7 +16882,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -16899,7 +17056,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -17129,7 +17286,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -17331,7 +17488,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -17533,7 +17690,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -17747,7 +17904,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -17963,7 +18120,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -18175,7 +18332,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -18387,7 +18544,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -18613,7 +18770,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -18787,7 +18944,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -18973,7 +19130,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -19171,7 +19328,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -19365,7 +19522,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -19551,7 +19708,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -19743,7 +19900,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -19937,7 +20094,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -20131,7 +20288,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -20313,7 +20470,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -20495,7 +20652,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -20689,7 +20846,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -20877,7 +21034,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -21071,7 +21228,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -21253,7 +21410,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -21298,7 +21455,7 @@
       <c r="AN25" s="11"/>
       <c r="AO25" s="11"/>
       <c r="AP25" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AQ25" s="11"/>
       <c r="AR25" s="11"/>
@@ -21437,7 +21594,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -21663,7 +21820,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -21845,7 +22002,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -22027,7 +22184,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -22227,7 +22384,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -22445,7 +22602,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -22633,7 +22790,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -22825,7 +22982,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -23017,7 +23174,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -23207,7 +23364,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -23397,7 +23554,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -23589,7 +23746,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -23781,7 +23938,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -23973,7 +24130,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -24075,7 +24232,7 @@
       <c r="CE39" s="11"/>
       <c r="CF39" s="12"/>
       <c r="CH39" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="CW39" s="10"/>
       <c r="CX39" s="11"/>
@@ -24166,7 +24323,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -24390,7 +24547,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -24490,7 +24647,7 @@
       <c r="CE41" s="11"/>
       <c r="CF41" s="12"/>
       <c r="CH41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="CW41" s="10"/>
       <c r="CX41" s="11"/>
@@ -24585,7 +24742,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -24719,7 +24876,7 @@
       <c r="CE42" s="11"/>
       <c r="CF42" s="12"/>
       <c r="CH42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="CW42" s="10"/>
       <c r="CX42" s="11"/>
@@ -24818,7 +24975,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -24938,7 +25095,7 @@
       <c r="CE43" s="11"/>
       <c r="CF43" s="12"/>
       <c r="CH43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="CW43" s="10"/>
       <c r="CX43" s="11"/>
@@ -25041,7 +25198,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -25243,7 +25400,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -25525,7 +25682,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -25703,7 +25860,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -25905,7 +26062,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -26077,7 +26234,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -26415,7 +26572,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -26753,7 +26910,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -27091,7 +27248,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -27429,7 +27586,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -27767,7 +27924,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>

</xml_diff>

<commit_message>
work on schematic and pcb
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="242">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -905,12 +905,6 @@
     <t>50 ms timer</t>
   </si>
   <si>
-    <t>Motor Driver</t>
-  </si>
-  <si>
-    <t>uController</t>
-  </si>
-  <si>
     <t>AIN1</t>
   </si>
   <si>
@@ -921,24 +915,6 @@
   </si>
   <si>
     <t>BIN2</t>
-  </si>
-  <si>
-    <t>PF2</t>
-  </si>
-  <si>
-    <t>PF3</t>
-  </si>
-  <si>
-    <t>Forward, right motor</t>
-  </si>
-  <si>
-    <t>Forward, left motor</t>
-  </si>
-  <si>
-    <t>Backward, right motor</t>
-  </si>
-  <si>
-    <t>Backward, left motor</t>
   </si>
   <si>
     <t>System config, study how to obtain more clock speeds</t>
@@ -1041,6 +1017,9 @@
   </si>
   <si>
     <t>Toggle PF2 and PF3 with PWM on / off, commanded by 2nd uC through CAN</t>
+  </si>
+  <si>
+    <t>GPIO</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1510,126 +1489,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1647,7 +1506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1751,19 +1610,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2375,61 +2226,6 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3295650</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6429375" y="4953000"/>
-          <a:ext cx="3295650" cy="971550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -5047,7 +4843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5304,27 +5100,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C25" s="60" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>177</v>
       </c>
       <c r="C26" s="60" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -5333,7 +5129,7 @@
         <v>177</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5342,7 +5138,7 @@
         <v>177</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5351,7 +5147,7 @@
         <v>177</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -5360,7 +5156,7 @@
         <v>177</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5386,7 +5182,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>164</v>
@@ -5397,29 +5193,29 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>164</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>164</v>
@@ -5443,18 +5239,18 @@
         <v>164</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>164</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -5471,7 +5267,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="62" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>174</v>
@@ -5486,7 +5282,7 @@
         <v>174</v>
       </c>
       <c r="C44" s="60" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -7041,10 +6837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7071,18 +6867,18 @@
       <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="75" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>170</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="76" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -7091,24 +6887,24 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="79"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="79"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="84"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
@@ -7121,16 +6917,16 @@
       <c r="E4" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="71" t="s">
         <v>59</v>
       </c>
       <c r="G4" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="81"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="84"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
@@ -7143,7 +6939,7 @@
       <c r="E5" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="71" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="46" t="s">
@@ -7152,21 +6948,21 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="72" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
@@ -7179,16 +6975,16 @@
       <c r="E7" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="71" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="H7" s="82"/>
+      <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="1" t="s">
         <v>47</v>
       </c>
@@ -7196,12 +6992,12 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>241</v>
       </c>
       <c r="E8" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="71" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="46" t="s">
@@ -7210,7 +7006,7 @@
       <c r="H8" s="58"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
@@ -7218,12 +7014,12 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>241</v>
       </c>
       <c r="E9" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="79" t="s">
+      <c r="F9" s="71" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="46" t="s">
@@ -7232,7 +7028,7 @@
       <c r="H9" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="76" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -7247,14 +7043,14 @@
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="71" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -7267,14 +7063,14 @@
       <c r="E12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="71" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="76" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -7289,14 +7085,16 @@
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="79" t="s">
+      <c r="F14" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="84"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -7309,14 +7107,16 @@
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="84" t="s">
+      <c r="A17" s="76" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -7331,14 +7131,14 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="79" t="s">
+      <c r="F17" s="71" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="84"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -7351,14 +7151,14 @@
       <c r="E18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F18" s="71" t="s">
         <v>151</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="84"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
@@ -7371,14 +7171,16 @@
       <c r="E19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
@@ -7391,14 +7193,16 @@
       <c r="E20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="79" t="s">
+      <c r="F20" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="84"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -7411,7 +7215,7 @@
       <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="79" t="s">
+      <c r="F21" s="71" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="1"/>
@@ -7434,62 +7238,6 @@
       </c>
       <c r="D24" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="76" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="77" t="s">
-        <v>222</v>
-      </c>
-      <c r="D28" s="78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="71" t="s">
-        <v>223</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="72" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="71" t="s">
-        <v>224</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D30" s="72" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="73" t="s">
-        <v>226</v>
-      </c>
-      <c r="C32" s="74" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="75" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -7923,7 +7671,7 @@
       <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="77" t="s">
         <v>115</v>
       </c>
       <c r="B5" s="47">
@@ -7944,19 +7692,19 @@
       <c r="G5" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="87" t="s">
-        <v>239</v>
-      </c>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="87"/>
+      <c r="I5" s="79" t="s">
+        <v>231</v>
+      </c>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -7980,14 +7728,14 @@
       <c r="G6" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="52"/>
@@ -7995,17 +7743,17 @@
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="79"/>
+      <c r="P7" s="79"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="78" t="s">
         <v>118</v>
       </c>
       <c r="B8" s="50">
@@ -8031,17 +7779,17 @@
       <c r="G8" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="87"/>
-      <c r="L8" s="87"/>
-      <c r="M8" s="87"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="87"/>
-      <c r="P8" s="87"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="79"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="79"/>
+      <c r="P8" s="79"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -8065,17 +7813,17 @@
       <c r="G9" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
-      <c r="O9" s="87"/>
-      <c r="P9" s="87"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
+      <c r="P9" s="79"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -8099,17 +7847,17 @@
       <c r="G10" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="87"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -8133,14 +7881,14 @@
       <c r="G11" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="87"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="87"/>
-      <c r="O11" s="87"/>
-      <c r="P11" s="87"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="79"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>
@@ -8148,17 +7896,17 @@
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="77" t="s">
         <v>123</v>
       </c>
       <c r="B13" s="47">
@@ -8179,17 +7927,17 @@
       <c r="G13" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="87"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="79"/>
+      <c r="P13" s="79"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="85"/>
+      <c r="A14" s="77"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -8213,17 +7961,17 @@
       <c r="G14" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="87"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="87"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
+      <c r="A15" s="77"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -8247,17 +7995,17 @@
       <c r="G15" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="79"/>
+      <c r="P15" s="79"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -8281,17 +8029,17 @@
       <c r="G16" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="87"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="87"/>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="87"/>
+      <c r="I16" s="79"/>
+      <c r="J16" s="79"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="79"/>
+      <c r="P16" s="79"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="77" t="s">
         <v>127</v>
       </c>
       <c r="B17" s="50">
@@ -8317,17 +8065,17 @@
       <c r="G17" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="87"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="79"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="79"/>
+      <c r="P17" s="79"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -8351,14 +8099,14 @@
       <c r="G18" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">

</xml_diff>

<commit_message>
added alternative dc motor supplier
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="244">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1020,6 +1020,12 @@
   </si>
   <si>
     <t>Bin2</t>
+  </si>
+  <si>
+    <t>Alternative motors</t>
+  </si>
+  <si>
+    <t>maxon dc motor</t>
   </si>
 </sst>
 </file>
@@ -6839,7 +6845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -7578,8 +7584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7610,6 +7616,9 @@
       <c r="G1" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="I1" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
@@ -7633,6 +7642,9 @@
       </c>
       <c r="G2" s="46" t="s">
         <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
temp sensor and light sensor 1
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="V_in" localSheetId="4">'Light sensor #2'!$B$5</definedName>
     <definedName name="V_in">'Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1312,11 +1312,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2103,11 +2103,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2144,16 +2154,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6976,7 +6976,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7008,9 +7008,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7042,6 +7043,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7217,21 +7219,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -7249,7 +7251,7 @@
       <c r="O1" s="62"/>
       <c r="P1" s="62"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="62"/>
       <c r="B2" s="61" t="s">
         <v>178</v>
@@ -7258,10 +7260,10 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="62"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
       <c r="B4" s="1" t="s">
         <v>175</v>
@@ -7273,7 +7275,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
       <c r="B5" s="1" t="s">
         <v>175</v>
@@ -7285,7 +7287,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="1" t="s">
         <v>175</v>
@@ -7297,7 +7299,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>
       <c r="B7" s="1" t="s">
         <v>175</v>
@@ -7309,7 +7311,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="62"/>
       <c r="B8" s="1" t="s">
         <v>175</v>
@@ -7321,7 +7323,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="62"/>
       <c r="B9" s="1" t="s">
         <v>175</v>
@@ -7330,7 +7332,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="62"/>
       <c r="B10" s="1" t="s">
         <v>175</v>
@@ -7339,7 +7341,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="62"/>
       <c r="B11" s="1" t="s">
         <v>175</v>
@@ -7348,7 +7350,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="62"/>
       <c r="B12" s="1" t="s">
         <v>175</v>
@@ -7358,7 +7360,7 @@
       </c>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="62"/>
       <c r="B13" s="1" t="s">
         <v>175</v>
@@ -7367,7 +7369,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="62"/>
       <c r="B14" s="1" t="s">
         <v>175</v>
@@ -7376,7 +7378,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="62"/>
       <c r="B15" s="1" t="s">
         <v>175</v>
@@ -7388,7 +7390,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="62"/>
       <c r="B16" s="1" t="s">
         <v>175</v>
@@ -7400,7 +7402,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="62"/>
       <c r="B17" s="46" t="s">
         <v>175</v>
@@ -7409,7 +7411,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="62"/>
       <c r="B18" s="46" t="s">
         <v>175</v>
@@ -7418,7 +7420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="62"/>
       <c r="B19" s="1" t="s">
         <v>175</v>
@@ -7430,7 +7432,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="62"/>
       <c r="B20" s="46" t="s">
         <v>175</v>
@@ -7439,7 +7441,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="62"/>
       <c r="B21" s="46" t="s">
         <v>175</v>
@@ -7451,7 +7453,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="62"/>
       <c r="B22" s="46" t="s">
         <v>175</v>
@@ -7460,7 +7462,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="62"/>
       <c r="B23" s="46" t="s">
         <v>175</v>
@@ -7469,7 +7471,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="62"/>
       <c r="B24" s="46" t="s">
         <v>175</v>
@@ -7478,7 +7480,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="62" t="s">
         <v>226</v>
       </c>
@@ -7489,7 +7491,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
         <v>226</v>
       </c>
@@ -7503,7 +7505,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="62"/>
       <c r="B27" s="1" t="s">
         <v>175</v>
@@ -7512,7 +7514,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="62"/>
       <c r="B28" s="1" t="s">
         <v>175</v>
@@ -7521,7 +7523,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="62"/>
       <c r="B29" s="1" t="s">
         <v>175</v>
@@ -7530,7 +7532,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="62"/>
       <c r="B30" s="1" t="s">
         <v>175</v>
@@ -7539,7 +7541,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="62"/>
       <c r="B31" s="1" t="s">
         <v>175</v>
@@ -7548,7 +7550,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="62"/>
       <c r="B32" s="1" t="s">
         <v>175</v>
@@ -7557,10 +7559,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="62"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="62"/>
       <c r="B34" s="1" t="s">
         <v>162</v>
@@ -7569,7 +7571,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="62"/>
       <c r="B35" s="1" t="s">
         <v>162</v>
@@ -7578,7 +7580,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="62" t="s">
         <v>227</v>
       </c>
@@ -7589,7 +7591,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>227</v>
       </c>
@@ -7600,7 +7602,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="62" t="s">
         <v>227</v>
       </c>
@@ -7611,7 +7613,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="62" t="s">
         <v>227</v>
       </c>
@@ -7622,7 +7624,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="62"/>
       <c r="B40" s="1" t="s">
         <v>162</v>
@@ -7631,7 +7633,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="62"/>
       <c r="B41" s="1" t="s">
         <v>162</v>
@@ -7640,7 +7642,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
         <v>227</v>
       </c>
@@ -7651,7 +7653,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="62"/>
       <c r="B43" s="1" t="s">
         <v>165</v>
@@ -7660,10 +7662,10 @@
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="62"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="62" t="s">
         <v>227</v>
       </c>
@@ -7674,7 +7676,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="62"/>
       <c r="B46" s="1" t="s">
         <v>172</v>
@@ -7683,7 +7685,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="62"/>
       <c r="B47" s="46" t="s">
         <v>172</v>
@@ -7692,47 +7694,47 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="62"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="62"/>
       <c r="B49" s="90"/>
       <c r="C49" s="90" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="62"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="62"/>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="62"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="62"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="62"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="62"/>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="62"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="62"/>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="62"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="62"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="62"/>
     </row>
   </sheetData>
@@ -7742,14 +7744,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -7817,7 +7819,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -7906,7 +7908,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7996,7 +7998,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -8086,7 +8088,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -8336,7 +8338,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -8454,7 +8456,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -8568,7 +8570,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -8680,7 +8682,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -8794,7 +8796,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -8906,7 +8908,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -9020,7 +9022,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -9180,7 +9182,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -9346,7 +9348,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -9510,7 +9512,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -9664,7 +9666,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -9818,7 +9820,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -9982,7 +9984,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -10150,7 +10152,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -10320,7 +10322,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -10472,7 +10474,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -10602,7 +10604,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -10718,7 +10720,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -10842,7 +10844,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -10966,7 +10968,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -11088,7 +11090,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -11208,7 +11210,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -11326,7 +11328,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -11440,7 +11442,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -11554,7 +11556,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -11664,7 +11666,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -11774,7 +11776,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -11884,7 +11886,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -11994,7 +11996,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -12104,7 +12106,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -12216,7 +12218,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -12330,7 +12332,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -12440,7 +12442,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -12550,7 +12552,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12657,7 +12659,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -12755,7 +12757,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -12844,7 +12846,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -12933,7 +12935,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -13022,7 +13024,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -13108,7 +13110,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -13194,7 +13196,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -13280,7 +13282,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -13366,7 +13368,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -13452,7 +13454,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -13790,7 +13792,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -14128,7 +14130,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -14466,7 +14468,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -14804,7 +14806,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -15142,7 +15144,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -15492,14 +15494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -15568,7 +15570,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15741,7 +15743,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -15915,7 +15917,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -16145,7 +16147,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -16347,7 +16349,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -16549,7 +16551,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -16763,7 +16765,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -16979,7 +16981,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -17191,7 +17193,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -17403,7 +17405,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -17629,7 +17631,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -17803,7 +17805,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -17989,7 +17991,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -18187,7 +18189,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -18381,7 +18383,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -18567,7 +18569,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -18759,7 +18761,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -18953,7 +18955,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -19147,7 +19149,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -19329,7 +19331,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -19511,7 +19513,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -19705,7 +19707,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -19893,7 +19895,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -20087,7 +20089,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -20269,7 +20271,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -20453,7 +20455,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -20679,7 +20681,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -20861,7 +20863,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -21043,7 +21045,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -21243,7 +21245,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -21461,7 +21463,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -21649,7 +21651,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -21841,7 +21843,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -22033,7 +22035,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -22223,7 +22225,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -22413,7 +22415,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -22605,7 +22607,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -22797,7 +22799,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -22989,7 +22991,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -23182,7 +23184,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -23406,7 +23408,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -23601,7 +23603,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -23834,7 +23836,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -24057,7 +24059,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -24259,7 +24261,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -24541,7 +24543,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -24719,7 +24721,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -24921,7 +24923,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -25093,7 +25095,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -25431,7 +25433,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -25769,7 +25771,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -26107,7 +26109,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -26445,7 +26447,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -26783,7 +26785,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -27428,14 +27430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="63" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="63" customWidth="1"/>
@@ -27451,7 +27453,7 @@
     <col min="40" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="65"/>
       <c r="B1" s="65"/>
       <c r="C1" s="66"/>
@@ -27488,7 +27490,7 @@
       <c r="AL1" s="66"/>
       <c r="AM1" s="66"/>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="65"/>
       <c r="B2" s="67"/>
       <c r="C2" s="67">
@@ -27537,7 +27539,7 @@
       <c r="AL2" s="67"/>
       <c r="AM2" s="66"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="65"/>
       <c r="B3" s="67">
         <v>1</v>
@@ -27596,7 +27598,7 @@
       <c r="AL3" s="67"/>
       <c r="AM3" s="66"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="65"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67">
@@ -27657,7 +27659,7 @@
       <c r="AL4" s="67"/>
       <c r="AM4" s="66"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="65"/>
       <c r="B5" s="67">
         <v>1</v>
@@ -27722,7 +27724,7 @@
       </c>
       <c r="AM5" s="66"/>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="65"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67">
@@ -27787,7 +27789,7 @@
       </c>
       <c r="AM6" s="66"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="65"/>
       <c r="B7" s="67">
         <v>1</v>
@@ -27854,7 +27856,7 @@
       <c r="AL7" s="67"/>
       <c r="AM7" s="66"/>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="65"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67">
@@ -27915,7 +27917,7 @@
       <c r="AL8" s="67"/>
       <c r="AM8" s="65"/>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="65"/>
       <c r="B9" s="67">
         <v>1</v>
@@ -27976,7 +27978,7 @@
       <c r="AL9" s="67"/>
       <c r="AM9" s="65"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="65"/>
       <c r="B10" s="65"/>
       <c r="C10" s="65"/>
@@ -28013,7 +28015,7 @@
       <c r="AL10" s="65"/>
       <c r="AM10" s="65"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12" s="64" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -28115,7 +28117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="65"/>
       <c r="B14" s="65"/>
       <c r="C14" s="66"/>
@@ -28152,7 +28154,7 @@
       <c r="AL14" s="66"/>
       <c r="AM14" s="66"/>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="65"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -28195,7 +28197,7 @@
       <c r="AL15" s="67"/>
       <c r="AM15" s="66"/>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="65"/>
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
@@ -28248,7 +28250,7 @@
       <c r="AL16" s="67"/>
       <c r="AM16" s="66"/>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="65"/>
       <c r="B17" s="67">
         <v>1</v>
@@ -28321,7 +28323,7 @@
       </c>
       <c r="AM17" s="66"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="65"/>
       <c r="B18" s="67"/>
       <c r="C18" s="67">
@@ -28384,7 +28386,7 @@
       </c>
       <c r="AM18" s="66"/>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="65"/>
       <c r="B19" s="67"/>
       <c r="C19" s="67"/>
@@ -28435,7 +28437,7 @@
       </c>
       <c r="AM19" s="66"/>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="65"/>
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
@@ -28488,7 +28490,7 @@
       </c>
       <c r="AM20" s="66"/>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="65"/>
       <c r="B21" s="67"/>
       <c r="C21" s="67">
@@ -28547,7 +28549,7 @@
       <c r="AL21" s="67"/>
       <c r="AM21" s="65"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="65"/>
       <c r="B22" s="67"/>
       <c r="C22" s="67"/>
@@ -28590,7 +28592,7 @@
       <c r="AL22" s="67"/>
       <c r="AM22" s="65"/>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="65"/>
       <c r="B23" s="65"/>
       <c r="C23" s="65"/>
@@ -28627,7 +28629,7 @@
       <c r="AL23" s="65"/>
       <c r="AM23" s="65"/>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B25" s="64" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -28815,20 +28817,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>190</v>
       </c>
@@ -28836,7 +28838,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>195</v>
       </c>
@@ -28850,7 +28852,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -28861,7 +28863,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>1</v>
       </c>
@@ -28872,7 +28874,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>191</v>
       </c>
@@ -28886,7 +28888,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L6">
         <v>3</v>
       </c>
@@ -28897,22 +28899,22 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L10">
         <v>7</v>
       </c>
@@ -28924,14 +28926,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
@@ -28942,7 +28944,7 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -28965,8 +28967,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="105" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="107" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -28979,8 +28981,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="105"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="107"/>
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
@@ -28991,8 +28993,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="105"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
       <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
@@ -29013,8 +29015,8 @@
       </c>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="105"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
       <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
@@ -29035,9 +29037,9 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="105"/>
-      <c r="B6" s="120" t="s">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="107"/>
+      <c r="B6" s="108" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="75" t="s">
@@ -29047,13 +29049,13 @@
       <c r="E6" s="75" t="s">
         <v>308</v>
       </c>
-      <c r="F6" s="119"/>
+      <c r="F6" s="105"/>
       <c r="G6" s="75"/>
       <c r="H6" s="75"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="105"/>
-      <c r="B7" s="121"/>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="107"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -29063,8 +29065,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="105"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
       <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
@@ -29085,8 +29087,8 @@
       </c>
       <c r="H8" s="73"/>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="105"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -29107,8 +29109,8 @@
       </c>
       <c r="H9" s="58"/>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="105"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
       <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
@@ -29129,52 +29131,52 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="105" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="106" t="s">
         <v>247</v>
       </c>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="106"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="106"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="105"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="105"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="107"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="106"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="106"/>
+      <c r="G14" s="106"/>
+      <c r="H14" s="106"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="105"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="107"/>
+      <c r="B15" s="106"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="105"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="107"/>
       <c r="B16" s="77" t="s">
         <v>243</v>
       </c>
@@ -29189,8 +29191,8 @@
       <c r="G16" s="77"/>
       <c r="H16" s="77"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="105"/>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="107"/>
       <c r="B17" s="77" t="s">
         <v>244</v>
       </c>
@@ -29200,15 +29202,15 @@
       <c r="D17" s="77" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="118" t="s">
+      <c r="E17" s="104" t="s">
         <v>293</v>
       </c>
       <c r="F17" s="103"/>
       <c r="G17" s="103"/>
       <c r="H17" s="77"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="105"/>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="107"/>
       <c r="B18" s="77" t="s">
         <v>33</v>
       </c>
@@ -29218,15 +29220,15 @@
       <c r="D18" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="118" t="s">
+      <c r="E18" s="104" t="s">
         <v>294</v>
       </c>
       <c r="F18" s="103"/>
       <c r="G18" s="103"/>
       <c r="H18" s="78"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="105"/>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="107"/>
       <c r="B19" s="77" t="s">
         <v>34</v>
       </c>
@@ -29245,8 +29247,8 @@
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="105" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="107" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -29269,8 +29271,8 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="105"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="107"/>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
@@ -29291,9 +29293,9 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="105"/>
-      <c r="B23" s="120" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="107"/>
+      <c r="B23" s="108" t="s">
         <v>307</v>
       </c>
       <c r="C23" s="75" t="s">
@@ -29303,13 +29305,13 @@
       <c r="E23" s="75" t="s">
         <v>309</v>
       </c>
-      <c r="F23" s="119"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="75"/>
       <c r="H23" s="75"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="105"/>
-      <c r="B24" s="121"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="107"/>
+      <c r="B24" s="109"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -29317,8 +29319,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="105"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="107"/>
       <c r="B25" s="1" t="s">
         <v>288</v>
       </c>
@@ -29339,11 +29341,11 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="105" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="107" t="s">
         <v>295</v>
       </c>
-      <c r="B27" s="120" t="s">
+      <c r="B27" s="108" t="s">
         <v>296</v>
       </c>
       <c r="C27" s="75" t="s">
@@ -29353,13 +29355,13 @@
       <c r="E27" s="75" t="s">
         <v>310</v>
       </c>
-      <c r="F27" s="119"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="75"/>
       <c r="H27" s="75"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="105"/>
-      <c r="B28" s="121"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="107"/>
+      <c r="B28" s="109"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -29367,8 +29369,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="105"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="107"/>
       <c r="B29" s="1" t="s">
         <v>297</v>
       </c>
@@ -29387,8 +29389,8 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="105"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="107"/>
       <c r="B30" s="1" t="s">
         <v>298</v>
       </c>
@@ -29407,8 +29409,8 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="105"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="107"/>
       <c r="B31" s="1" t="s">
         <v>299</v>
       </c>
@@ -29427,8 +29429,8 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33" s="105" t="s">
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="107" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -29449,8 +29451,8 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
-      <c r="A34" s="105"/>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="107"/>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -29469,8 +29471,8 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="105"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="107"/>
       <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
@@ -29491,8 +29493,8 @@
       </c>
       <c r="H35" s="75"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="105"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="107"/>
       <c r="B36" s="4" t="s">
         <v>10</v>
       </c>
@@ -29513,8 +29515,8 @@
       </c>
       <c r="H36" s="102"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="105"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="107"/>
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
@@ -29533,7 +29535,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -29544,7 +29546,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>18</v>
       </c>
@@ -29571,14 +29573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29587,7 +29589,7 @@
     <col min="12" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -29604,22 +29606,22 @@
       <c r="E1" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="116" t="s">
         <v>256</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="106" t="s">
+      <c r="J1" s="117"/>
+      <c r="K1" s="110" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="111" t="s">
+      <c r="L1" s="115" t="s">
         <v>276</v>
       </c>
-      <c r="M1" s="111"/>
+      <c r="M1" s="115"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -29636,14 +29638,14 @@
       <c r="E2" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="110"/>
+      <c r="H2" s="114"/>
       <c r="I2" s="84" t="s">
         <v>272</v>
       </c>
       <c r="J2" s="84" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="107"/>
+      <c r="K2" s="111"/>
       <c r="L2" s="84" t="s">
         <v>272</v>
       </c>
@@ -29651,7 +29653,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>251</v>
       </c>
@@ -29671,20 +29673,20 @@
       <c r="H3" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="116" t="s">
         <v>264</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="112" t="s">
+      <c r="J3" s="117"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="M3" s="113"/>
+      <c r="M3" s="117"/>
       <c r="P3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>252</v>
       </c>
@@ -29725,7 +29727,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>253</v>
       </c>
@@ -29758,7 +29760,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H6" s="76">
         <v>10.75</v>
       </c>
@@ -29785,7 +29787,7 @@
       </c>
       <c r="Q6" s="89"/>
     </row>
-    <row r="7" spans="1:17" ht="18">
+    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>255</v>
       </c>
@@ -29821,7 +29823,7 @@
       </c>
       <c r="Q7" s="90"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H8" s="76">
         <v>107.53</v>
       </c>
@@ -29843,7 +29845,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>257</v>
       </c>
@@ -29874,7 +29876,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -29905,7 +29907,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H11" s="76">
         <v>107527</v>
       </c>
@@ -29948,14 +29950,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29964,7 +29966,7 @@
     <col min="12" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -29981,26 +29983,26 @@
       <c r="E1" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="116" t="s">
         <v>256</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="106" t="s">
+      <c r="J1" s="117"/>
+      <c r="K1" s="110" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="111" t="s">
+      <c r="L1" s="115" t="s">
         <v>286</v>
       </c>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111" t="s">
+      <c r="M1" s="115"/>
+      <c r="N1" s="115" t="s">
         <v>281</v>
       </c>
-      <c r="O1" s="111"/>
+      <c r="O1" s="115"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -30017,14 +30019,14 @@
       <c r="E2" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="110"/>
+      <c r="H2" s="114"/>
       <c r="I2" s="84" t="s">
         <v>272</v>
       </c>
       <c r="J2" s="84" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="107"/>
+      <c r="K2" s="111"/>
       <c r="L2" s="84" t="s">
         <v>279</v>
       </c>
@@ -30038,7 +30040,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>282</v>
       </c>
@@ -30058,22 +30060,22 @@
       <c r="H3" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="116" t="s">
         <v>264</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="112" t="s">
+      <c r="J3" s="117"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="116" t="s">
         <v>254</v>
       </c>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="113"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="117"/>
       <c r="T3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>283</v>
       </c>
@@ -30122,7 +30124,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18">
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>253</v>
       </c>
@@ -30163,7 +30165,7 @@
         <v>9.6116504854368928E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H6" s="76">
         <v>10.75</v>
       </c>
@@ -30198,7 +30200,7 @@
       </c>
       <c r="U6" s="89"/>
     </row>
-    <row r="7" spans="1:21" ht="18">
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>255</v>
       </c>
@@ -30242,7 +30244,7 @@
       </c>
       <c r="U7" s="90"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H8" s="76">
         <v>107.53</v>
       </c>
@@ -30272,7 +30274,7 @@
         <v>2.9117647058823528</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>257</v>
       </c>
@@ -30311,7 +30313,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -30350,7 +30352,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H11" s="76">
         <v>107527</v>
       </c>
@@ -30380,7 +30382,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L12" s="101" t="s">
         <v>287</v>
       </c>
@@ -30388,7 +30390,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N13" s="100" t="s">
         <v>287</v>
       </c>
@@ -30418,26 +30420,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -30449,14 +30451,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -30468,7 +30470,7 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>104</v>
       </c>
@@ -30503,7 +30505,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>103</v>
       </c>
@@ -30544,7 +30546,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>99</v>
       </c>
@@ -30585,7 +30587,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>92</v>
       </c>
@@ -30626,13 +30628,13 @@
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>85</v>
       </c>
@@ -30648,7 +30650,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>83</v>
       </c>
@@ -30665,7 +30667,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>194</v>
       </c>
@@ -30673,22 +30675,22 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -30709,7 +30711,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -30727,7 +30729,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>187</v>
       </c>
@@ -30739,14 +30741,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -30755,7 +30757,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
@@ -30775,7 +30777,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>110</v>
       </c>
@@ -30799,7 +30801,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>112</v>
       </c>
@@ -30827,15 +30829,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
-      <c r="A5" s="115" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="119" t="s">
         <v>113</v>
       </c>
       <c r="B5" s="47">
@@ -30856,19 +30858,19 @@
       <c r="G5" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="121" t="s">
         <v>229</v>
       </c>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="115"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="119"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -30892,32 +30894,32 @@
       <c r="G6" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="116" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="120" t="s">
         <v>116</v>
       </c>
       <c r="B8" s="50">
@@ -30943,17 +30945,17 @@
       <c r="G8" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="116"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="120"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -30977,17 +30979,17 @@
       <c r="G9" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="116"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="120"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -31011,17 +31013,17 @@
       <c r="G10" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="121"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="121"/>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="116"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="120"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -31045,32 +31047,32 @@
       <c r="G11" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="117"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="117"/>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="115" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="119" t="s">
         <v>121</v>
       </c>
       <c r="B13" s="47">
@@ -31091,17 +31093,17 @@
       <c r="G13" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I13" s="117"/>
-      <c r="J13" s="117"/>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="115"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="119"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -31125,17 +31127,17 @@
       <c r="G14" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="I14" s="117"/>
-      <c r="J14" s="117"/>
-      <c r="K14" s="117"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="121"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="121"/>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="115"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="119"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -31159,17 +31161,17 @@
       <c r="G15" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="117"/>
-      <c r="J15" s="117"/>
-      <c r="K15" s="117"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-      <c r="N15" s="117"/>
-      <c r="O15" s="117"/>
-      <c r="P15" s="117"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="115"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="119"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -31193,17 +31195,17 @@
       <c r="G16" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="117"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="117"/>
-      <c r="P16" s="117"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="115" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="119" t="s">
         <v>125</v>
       </c>
       <c r="B17" s="50">
@@ -31229,17 +31231,17 @@
       <c r="G17" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="I17" s="117"/>
-      <c r="J17" s="117"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="117"/>
-      <c r="O17" s="117"/>
-      <c r="P17" s="117"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="115"/>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="119"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -31263,16 +31265,16 @@
       <c r="G18" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="117"/>
-      <c r="P18" s="117"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="121"/>
+      <c r="P18" s="121"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>128</v>
       </c>
@@ -31289,22 +31291,22 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -31312,7 +31314,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>136</v>
       </c>
@@ -31335,14 +31337,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="F2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -31410,7 +31412,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -31449,7 +31451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -31486,7 +31488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1">
+    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -31523,7 +31525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1">
+    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -31550,7 +31552,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1">
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -31574,7 +31576,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1">
+    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>69</v>
@@ -31596,7 +31598,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -31631,7 +31633,7 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adc light sensor input updates
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
@@ -32,12 +32,12 @@
     <definedName name="V_in" localSheetId="4">'Light sensor #2'!$B$5</definedName>
     <definedName name="V_in">'Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="311">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1291,45 +1291,34 @@
     <t>Center photocell input (reference)</t>
   </si>
   <si>
-    <t>Test adc</t>
-  </si>
-  <si>
     <t>PD6</t>
   </si>
   <si>
-    <t>Left LED</t>
+    <t>Create port and pin mapping defines</t>
   </si>
   <si>
-    <t>Right LED</t>
+    <t>ADC1 - Sequencer 3 - Chanel 0</t>
   </si>
   <si>
-    <t>Center LED</t>
+    <t>ADC1 - Sequencer 2 - Chanel 2</t>
   </si>
   <si>
-    <t>Create port and pin mapping defines</t>
+    <t>ADC1 - Sequencer 1 - Chanel 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1922,26 +1911,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1951,62 +1940,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
@@ -2019,19 +2008,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2045,13 +2034,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2076,7 +2065,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2088,7 +2077,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -2099,18 +2088,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2119,31 +2107,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2152,7 +2140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6976,7 +6964,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7008,10 +6996,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7043,7 +7030,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7219,21 +7205,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -7251,7 +7237,7 @@
       <c r="O1" s="62"/>
       <c r="P1" s="62"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="62"/>
       <c r="B2" s="61" t="s">
         <v>178</v>
@@ -7260,10 +7246,10 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="62"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="62"/>
       <c r="B4" s="1" t="s">
         <v>175</v>
@@ -7275,7 +7261,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="62"/>
       <c r="B5" s="1" t="s">
         <v>175</v>
@@ -7287,7 +7273,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="62"/>
       <c r="B6" s="1" t="s">
         <v>175</v>
@@ -7299,7 +7285,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="62"/>
       <c r="B7" s="1" t="s">
         <v>175</v>
@@ -7311,7 +7297,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="62"/>
       <c r="B8" s="1" t="s">
         <v>175</v>
@@ -7323,7 +7309,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="62"/>
       <c r="B9" s="1" t="s">
         <v>175</v>
@@ -7332,7 +7318,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="62"/>
       <c r="B10" s="1" t="s">
         <v>175</v>
@@ -7341,7 +7327,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="62"/>
       <c r="B11" s="1" t="s">
         <v>175</v>
@@ -7350,7 +7336,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="62"/>
       <c r="B12" s="1" t="s">
         <v>175</v>
@@ -7360,7 +7346,7 @@
       </c>
       <c r="E12" s="59"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="62"/>
       <c r="B13" s="1" t="s">
         <v>175</v>
@@ -7369,7 +7355,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="62"/>
       <c r="B14" s="1" t="s">
         <v>175</v>
@@ -7378,7 +7364,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="62"/>
       <c r="B15" s="1" t="s">
         <v>175</v>
@@ -7390,7 +7376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="62"/>
       <c r="B16" s="1" t="s">
         <v>175</v>
@@ -7402,7 +7388,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="62"/>
       <c r="B17" s="46" t="s">
         <v>175</v>
@@ -7411,7 +7397,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="62"/>
       <c r="B18" s="46" t="s">
         <v>175</v>
@@ -7420,7 +7406,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="62"/>
       <c r="B19" s="1" t="s">
         <v>175</v>
@@ -7432,7 +7418,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="62"/>
       <c r="B20" s="46" t="s">
         <v>175</v>
@@ -7441,7 +7427,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="62"/>
       <c r="B21" s="46" t="s">
         <v>175</v>
@@ -7453,7 +7439,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="62"/>
       <c r="B22" s="46" t="s">
         <v>175</v>
@@ -7462,7 +7448,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="62"/>
       <c r="B23" s="46" t="s">
         <v>175</v>
@@ -7471,7 +7457,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="62"/>
       <c r="B24" s="46" t="s">
         <v>175</v>
@@ -7480,7 +7466,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="62" t="s">
         <v>226</v>
       </c>
@@ -7491,7 +7477,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="62" t="s">
         <v>226</v>
       </c>
@@ -7505,7 +7491,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="62"/>
       <c r="B27" s="1" t="s">
         <v>175</v>
@@ -7514,7 +7500,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="62"/>
       <c r="B28" s="1" t="s">
         <v>175</v>
@@ -7523,7 +7509,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="62"/>
       <c r="B29" s="1" t="s">
         <v>175</v>
@@ -7532,7 +7518,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="62"/>
       <c r="B30" s="1" t="s">
         <v>175</v>
@@ -7541,7 +7527,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="62"/>
       <c r="B31" s="1" t="s">
         <v>175</v>
@@ -7550,7 +7536,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="62"/>
       <c r="B32" s="1" t="s">
         <v>175</v>
@@ -7559,10 +7545,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="62"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="62"/>
       <c r="B34" s="1" t="s">
         <v>162</v>
@@ -7571,7 +7557,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="62"/>
       <c r="B35" s="1" t="s">
         <v>162</v>
@@ -7580,7 +7566,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="62" t="s">
         <v>227</v>
       </c>
@@ -7591,7 +7577,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="62" t="s">
         <v>227</v>
       </c>
@@ -7602,7 +7588,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="62" t="s">
         <v>227</v>
       </c>
@@ -7613,7 +7599,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="62" t="s">
         <v>227</v>
       </c>
@@ -7624,7 +7610,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="62"/>
       <c r="B40" s="1" t="s">
         <v>162</v>
@@ -7633,7 +7619,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="62"/>
       <c r="B41" s="1" t="s">
         <v>162</v>
@@ -7642,7 +7628,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="62" t="s">
         <v>227</v>
       </c>
@@ -7653,7 +7639,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="62"/>
       <c r="B43" s="1" t="s">
         <v>165</v>
@@ -7662,10 +7648,10 @@
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="62"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="62" t="s">
         <v>227</v>
       </c>
@@ -7676,7 +7662,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="62"/>
       <c r="B46" s="1" t="s">
         <v>172</v>
@@ -7685,7 +7671,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="62"/>
       <c r="B47" s="46" t="s">
         <v>172</v>
@@ -7694,47 +7680,47 @@
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="62"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" s="62"/>
       <c r="B49" s="90"/>
       <c r="C49" s="90" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="62"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="62"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="62"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="62"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="62"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="62"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="62"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" s="62"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="62"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="62"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="62"/>
     </row>
   </sheetData>
@@ -7744,14 +7730,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -7819,7 +7805,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -7908,7 +7894,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7998,7 +7984,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -8088,7 +8074,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -8212,7 +8198,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -8338,7 +8324,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -8456,7 +8442,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -8570,7 +8556,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -8682,7 +8668,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -8796,7 +8782,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -8908,7 +8894,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -9022,7 +9008,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -9182,7 +9168,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -9348,7 +9334,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -9512,7 +9498,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -9666,7 +9652,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -9820,7 +9806,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -9984,7 +9970,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -10152,7 +10138,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -10322,7 +10308,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -10474,7 +10460,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -10604,7 +10590,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -10720,7 +10706,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -10844,7 +10830,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -10968,7 +10954,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -11090,7 +11076,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -11210,7 +11196,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -11328,7 +11314,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -11442,7 +11428,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -11556,7 +11542,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -11666,7 +11652,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -11776,7 +11762,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -11886,7 +11872,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -11996,7 +11982,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -12106,7 +12092,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -12218,7 +12204,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -12332,7 +12318,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -12442,7 +12428,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -12552,7 +12538,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12659,7 +12645,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -12757,7 +12743,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -12846,7 +12832,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -12935,7 +12921,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -13024,7 +13010,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -13110,7 +13096,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -13196,7 +13182,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -13282,7 +13268,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -13368,7 +13354,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -13454,7 +13440,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -13792,7 +13778,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -14130,7 +14116,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -14468,7 +14454,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -14806,7 +14792,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -15144,7 +15130,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -15494,14 +15480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -15570,7 +15556,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15743,7 +15729,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -15917,7 +15903,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -16147,7 +16133,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -16349,7 +16335,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -16551,7 +16537,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -16765,7 +16751,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -16981,7 +16967,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -17193,7 +17179,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -17405,7 +17391,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -17631,7 +17617,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -17805,7 +17791,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -17991,7 +17977,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -18189,7 +18175,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -18383,7 +18369,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -18569,7 +18555,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -18761,7 +18747,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -18955,7 +18941,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -19149,7 +19135,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -19331,7 +19317,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -19513,7 +19499,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -19707,7 +19693,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -19895,7 +19881,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -20089,7 +20075,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -20271,7 +20257,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -20455,7 +20441,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -20681,7 +20667,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -20863,7 +20849,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -21045,7 +21031,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -21245,7 +21231,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -21463,7 +21449,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -21651,7 +21637,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -21843,7 +21829,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -22035,7 +22021,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -22225,7 +22211,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -22415,7 +22401,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -22607,7 +22593,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -22799,7 +22785,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -22991,7 +22977,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -23184,7 +23170,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -23408,7 +23394,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -23603,7 +23589,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -23836,7 +23822,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -24059,7 +24045,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -24261,7 +24247,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -24543,7 +24529,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -24721,7 +24707,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -24923,7 +24909,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -25095,7 +25081,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -25433,7 +25419,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -25771,7 +25757,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -26109,7 +26095,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -26447,7 +26433,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -26785,7 +26771,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -27430,14 +27416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="63" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="63" customWidth="1"/>
@@ -27453,7 +27439,7 @@
     <col min="40" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39">
       <c r="A1" s="65"/>
       <c r="B1" s="65"/>
       <c r="C1" s="66"/>
@@ -27490,7 +27476,7 @@
       <c r="AL1" s="66"/>
       <c r="AM1" s="66"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39">
       <c r="A2" s="65"/>
       <c r="B2" s="67"/>
       <c r="C2" s="67">
@@ -27539,7 +27525,7 @@
       <c r="AL2" s="67"/>
       <c r="AM2" s="66"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39">
       <c r="A3" s="65"/>
       <c r="B3" s="67">
         <v>1</v>
@@ -27598,7 +27584,7 @@
       <c r="AL3" s="67"/>
       <c r="AM3" s="66"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39">
       <c r="A4" s="65"/>
       <c r="B4" s="67"/>
       <c r="C4" s="67">
@@ -27659,7 +27645,7 @@
       <c r="AL4" s="67"/>
       <c r="AM4" s="66"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39">
       <c r="A5" s="65"/>
       <c r="B5" s="67">
         <v>1</v>
@@ -27724,7 +27710,7 @@
       </c>
       <c r="AM5" s="66"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39">
       <c r="A6" s="65"/>
       <c r="B6" s="67"/>
       <c r="C6" s="67">
@@ -27789,7 +27775,7 @@
       </c>
       <c r="AM6" s="66"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39">
       <c r="A7" s="65"/>
       <c r="B7" s="67">
         <v>1</v>
@@ -27856,7 +27842,7 @@
       <c r="AL7" s="67"/>
       <c r="AM7" s="66"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39">
       <c r="A8" s="65"/>
       <c r="B8" s="67"/>
       <c r="C8" s="67">
@@ -27917,7 +27903,7 @@
       <c r="AL8" s="67"/>
       <c r="AM8" s="65"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39">
       <c r="A9" s="65"/>
       <c r="B9" s="67">
         <v>1</v>
@@ -27978,7 +27964,7 @@
       <c r="AL9" s="67"/>
       <c r="AM9" s="65"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39">
       <c r="A10" s="65"/>
       <c r="B10" s="65"/>
       <c r="C10" s="65"/>
@@ -28015,7 +28001,7 @@
       <c r="AL10" s="65"/>
       <c r="AM10" s="65"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39">
       <c r="B12" s="64" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -28117,7 +28103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39">
       <c r="A14" s="65"/>
       <c r="B14" s="65"/>
       <c r="C14" s="66"/>
@@ -28154,7 +28140,7 @@
       <c r="AL14" s="66"/>
       <c r="AM14" s="66"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39">
       <c r="A15" s="65"/>
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
@@ -28197,7 +28183,7 @@
       <c r="AL15" s="67"/>
       <c r="AM15" s="66"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39">
       <c r="A16" s="65"/>
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
@@ -28250,7 +28236,7 @@
       <c r="AL16" s="67"/>
       <c r="AM16" s="66"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39">
       <c r="A17" s="65"/>
       <c r="B17" s="67">
         <v>1</v>
@@ -28323,7 +28309,7 @@
       </c>
       <c r="AM17" s="66"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39">
       <c r="A18" s="65"/>
       <c r="B18" s="67"/>
       <c r="C18" s="67">
@@ -28386,7 +28372,7 @@
       </c>
       <c r="AM18" s="66"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39">
       <c r="A19" s="65"/>
       <c r="B19" s="67"/>
       <c r="C19" s="67"/>
@@ -28437,7 +28423,7 @@
       </c>
       <c r="AM19" s="66"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39">
       <c r="A20" s="65"/>
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
@@ -28490,7 +28476,7 @@
       </c>
       <c r="AM20" s="66"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39">
       <c r="A21" s="65"/>
       <c r="B21" s="67"/>
       <c r="C21" s="67">
@@ -28549,7 +28535,7 @@
       <c r="AL21" s="67"/>
       <c r="AM21" s="65"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39">
       <c r="A22" s="65"/>
       <c r="B22" s="67"/>
       <c r="C22" s="67"/>
@@ -28592,7 +28578,7 @@
       <c r="AL22" s="67"/>
       <c r="AM22" s="65"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39">
       <c r="A23" s="65"/>
       <c r="B23" s="65"/>
       <c r="C23" s="65"/>
@@ -28629,7 +28615,7 @@
       <c r="AL23" s="65"/>
       <c r="AM23" s="65"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39">
       <c r="B25" s="64" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -28817,20 +28803,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="69" t="s">
         <v>190</v>
       </c>
@@ -28838,7 +28824,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>195</v>
       </c>
@@ -28852,7 +28838,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -28863,7 +28849,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="L4">
         <v>1</v>
       </c>
@@ -28874,7 +28860,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="69" t="s">
         <v>191</v>
       </c>
@@ -28888,7 +28874,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="L6">
         <v>3</v>
       </c>
@@ -28899,22 +28885,22 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="L7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="L8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="L9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="L10">
         <v>7</v>
       </c>
@@ -28926,14 +28912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
@@ -28944,7 +28930,7 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -28967,8 +28953,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="106" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -28981,8 +28967,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="107"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="106"/>
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
@@ -28993,8 +28979,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="106"/>
       <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
@@ -29015,8 +29001,8 @@
       </c>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="106"/>
       <c r="B5" s="1" t="s">
         <v>42</v>
       </c>
@@ -29037,25 +29023,21 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
-      <c r="B6" s="108" t="s">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="A6" s="106"/>
+      <c r="B6" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="75" t="s">
-        <v>306</v>
-      </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75" t="s">
-        <v>308</v>
-      </c>
-      <c r="F6" s="105"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="109"/>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="106"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -29065,8 +29047,8 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="106"/>
       <c r="B8" s="1" t="s">
         <v>44</v>
       </c>
@@ -29087,8 +29069,8 @@
       </c>
       <c r="H8" s="73"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="106"/>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -29109,8 +29091,8 @@
       </c>
       <c r="H9" s="58"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
+    <row r="10" spans="1:8">
+      <c r="A10" s="106"/>
       <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
@@ -29131,52 +29113,52 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="107" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="105" t="s">
         <v>247</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="106"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="106"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="106"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
+    <row r="14" spans="1:8">
+      <c r="A14" s="106"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
+    <row r="15" spans="1:8">
+      <c r="A15" s="106"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="A16" s="106"/>
       <c r="B16" s="77" t="s">
         <v>243</v>
       </c>
@@ -29191,8 +29173,8 @@
       <c r="G16" s="77"/>
       <c r="H16" s="77"/>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+    <row r="17" spans="1:8" ht="15" customHeight="1">
+      <c r="A17" s="106"/>
       <c r="B17" s="77" t="s">
         <v>244</v>
       </c>
@@ -29209,8 +29191,8 @@
       <c r="G17" s="103"/>
       <c r="H17" s="77"/>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="107"/>
+    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="A18" s="106"/>
       <c r="B18" s="77" t="s">
         <v>33</v>
       </c>
@@ -29227,8 +29209,8 @@
       <c r="G18" s="103"/>
       <c r="H18" s="78"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
+    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="A19" s="106"/>
       <c r="B19" s="77" t="s">
         <v>34</v>
       </c>
@@ -29247,8 +29229,8 @@
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="107" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" s="106" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -29271,8 +29253,8 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
+    <row r="22" spans="1:8">
+      <c r="A22" s="106"/>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
@@ -29293,25 +29275,21 @@
       </c>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
-      <c r="B23" s="108" t="s">
-        <v>307</v>
-      </c>
-      <c r="C23" s="75" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" s="106"/>
+      <c r="B23" s="107" t="s">
         <v>306</v>
       </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75" t="s">
-        <v>309</v>
-      </c>
-      <c r="F23" s="105"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
-      <c r="B24" s="109"/>
+    <row r="24" spans="1:8">
+      <c r="A24" s="106"/>
+      <c r="B24" s="108"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -29319,8 +29297,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
+    <row r="25" spans="1:8">
+      <c r="A25" s="106"/>
       <c r="B25" s="1" t="s">
         <v>288</v>
       </c>
@@ -29341,27 +29319,23 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="107" t="s">
+    <row r="27" spans="1:8">
+      <c r="A27" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="107" t="s">
         <v>296</v>
       </c>
-      <c r="C27" s="75" t="s">
-        <v>306</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75" t="s">
-        <v>310</v>
-      </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="107"/>
-      <c r="B28" s="109"/>
+    <row r="28" spans="1:8">
+      <c r="A28" s="106"/>
+      <c r="B28" s="108"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -29369,8 +29343,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
+    <row r="29" spans="1:8">
+      <c r="A29" s="106"/>
       <c r="B29" s="1" t="s">
         <v>297</v>
       </c>
@@ -29383,14 +29357,16 @@
       <c r="E29" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="G29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
+    <row r="30" spans="1:8">
+      <c r="A30" s="106"/>
       <c r="B30" s="1" t="s">
         <v>298</v>
       </c>
@@ -29403,14 +29379,16 @@
       <c r="E30" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
+    <row r="31" spans="1:8">
+      <c r="A31" s="106"/>
       <c r="B31" s="1" t="s">
         <v>299</v>
       </c>
@@ -29423,14 +29401,16 @@
       <c r="E31" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="G31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="107" t="s">
+    <row r="33" spans="1:8" ht="15" customHeight="1">
+      <c r="A33" s="106" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -29451,8 +29431,8 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="107"/>
+    <row r="34" spans="1:8" ht="15" customHeight="1">
+      <c r="A34" s="106"/>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
@@ -29471,8 +29451,8 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="107"/>
+    <row r="35" spans="1:8">
+      <c r="A35" s="106"/>
       <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
@@ -29493,8 +29473,8 @@
       </c>
       <c r="H35" s="75"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
+    <row r="36" spans="1:8">
+      <c r="A36" s="106"/>
       <c r="B36" s="4" t="s">
         <v>10</v>
       </c>
@@ -29515,8 +29495,8 @@
       </c>
       <c r="H36" s="102"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
+    <row r="37" spans="1:8">
+      <c r="A37" s="106"/>
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
@@ -29535,7 +29515,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -29546,7 +29526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="C40" t="s">
         <v>18</v>
       </c>
@@ -29573,14 +29553,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29589,7 +29569,7 @@
     <col min="12" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -29606,22 +29586,22 @@
       <c r="E1" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="115" t="s">
         <v>256</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="110" t="s">
+      <c r="J1" s="116"/>
+      <c r="K1" s="109" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="115" t="s">
+      <c r="L1" s="114" t="s">
         <v>276</v>
       </c>
-      <c r="M1" s="115"/>
+      <c r="M1" s="114"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -29638,14 +29618,14 @@
       <c r="E2" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="114"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="84" t="s">
         <v>272</v>
       </c>
       <c r="J2" s="84" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="111"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="84" t="s">
         <v>272</v>
       </c>
@@ -29653,7 +29633,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>251</v>
       </c>
@@ -29673,20 +29653,20 @@
       <c r="H3" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="I3" s="115" t="s">
         <v>264</v>
       </c>
-      <c r="J3" s="117"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="116" t="s">
+      <c r="J3" s="116"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="115" t="s">
         <v>254</v>
       </c>
-      <c r="M3" s="117"/>
+      <c r="M3" s="116"/>
       <c r="P3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>252</v>
       </c>
@@ -29727,7 +29707,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="18">
       <c r="A5" s="1" t="s">
         <v>253</v>
       </c>
@@ -29760,7 +29740,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="H6" s="76">
         <v>10.75</v>
       </c>
@@ -29787,7 +29767,7 @@
       </c>
       <c r="Q6" s="89"/>
     </row>
-    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="18">
       <c r="A7" s="1" t="s">
         <v>255</v>
       </c>
@@ -29823,7 +29803,7 @@
       </c>
       <c r="Q7" s="90"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="H8" s="76">
         <v>107.53</v>
       </c>
@@ -29845,7 +29825,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>257</v>
       </c>
@@ -29876,7 +29856,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -29907,7 +29887,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="H11" s="76">
         <v>107527</v>
       </c>
@@ -29950,14 +29930,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29966,7 +29946,7 @@
     <col min="12" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -29983,26 +29963,26 @@
       <c r="E1" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="115" t="s">
         <v>256</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="110" t="s">
+      <c r="J1" s="116"/>
+      <c r="K1" s="109" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="115" t="s">
+      <c r="L1" s="114" t="s">
         <v>286</v>
       </c>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115" t="s">
+      <c r="M1" s="114"/>
+      <c r="N1" s="114" t="s">
         <v>281</v>
       </c>
-      <c r="O1" s="115"/>
+      <c r="O1" s="114"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>250</v>
       </c>
@@ -30019,14 +29999,14 @@
       <c r="E2" s="81" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="114"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="84" t="s">
         <v>272</v>
       </c>
       <c r="J2" s="84" t="s">
         <v>273</v>
       </c>
-      <c r="K2" s="111"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="84" t="s">
         <v>279</v>
       </c>
@@ -30040,7 +30020,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>282</v>
       </c>
@@ -30060,22 +30040,22 @@
       <c r="H3" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="I3" s="116" t="s">
+      <c r="I3" s="115" t="s">
         <v>264</v>
       </c>
-      <c r="J3" s="117"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="116" t="s">
+      <c r="J3" s="116"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="115" t="s">
         <v>254</v>
       </c>
-      <c r="M3" s="118"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="116"/>
       <c r="T3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>283</v>
       </c>
@@ -30124,7 +30104,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="1" t="s">
         <v>253</v>
       </c>
@@ -30165,7 +30145,7 @@
         <v>9.6116504854368928E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="H6" s="76">
         <v>10.75</v>
       </c>
@@ -30200,7 +30180,7 @@
       </c>
       <c r="U6" s="89"/>
     </row>
-    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="18">
       <c r="A7" s="1" t="s">
         <v>255</v>
       </c>
@@ -30244,7 +30224,7 @@
       </c>
       <c r="U7" s="90"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="H8" s="76">
         <v>107.53</v>
       </c>
@@ -30274,7 +30254,7 @@
         <v>2.9117647058823528</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>257</v>
       </c>
@@ -30313,7 +30293,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>259</v>
       </c>
@@ -30352,7 +30332,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="H11" s="76">
         <v>107527</v>
       </c>
@@ -30382,7 +30362,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="L12" s="101" t="s">
         <v>287</v>
       </c>
@@ -30390,7 +30370,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="N13" s="100" t="s">
         <v>287</v>
       </c>
@@ -30420,26 +30400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A13:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -30451,14 +30431,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -30470,7 +30450,7 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="36" t="s">
         <v>104</v>
       </c>
@@ -30505,7 +30485,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="36" t="s">
         <v>103</v>
       </c>
@@ -30546,7 +30526,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="36" t="s">
         <v>99</v>
       </c>
@@ -30587,7 +30567,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="36" t="s">
         <v>92</v>
       </c>
@@ -30628,13 +30608,13 @@
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="30" t="s">
         <v>85</v>
       </c>
@@ -30650,7 +30630,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="30" t="s">
         <v>83</v>
       </c>
@@ -30667,7 +30647,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="D8" t="s">
         <v>194</v>
       </c>
@@ -30675,22 +30655,22 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="26" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -30711,7 +30691,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -30729,7 +30709,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="E20" t="s">
         <v>187</v>
       </c>
@@ -30741,14 +30721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -30757,7 +30737,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
@@ -30777,7 +30757,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="46" t="s">
         <v>110</v>
       </c>
@@ -30801,7 +30781,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="46" t="s">
         <v>112</v>
       </c>
@@ -30829,15 +30809,15 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="119" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
+      <c r="A5" s="118" t="s">
         <v>113</v>
       </c>
       <c r="B5" s="47">
@@ -30858,19 +30838,19 @@
       <c r="G5" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="I5" s="121" t="s">
+      <c r="I5" s="120" t="s">
         <v>229</v>
       </c>
-      <c r="J5" s="121"/>
-      <c r="K5" s="121"/>
-      <c r="L5" s="121"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="121"/>
-      <c r="O5" s="121"/>
-      <c r="P5" s="121"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="119"/>
+    <row r="6" spans="1:16">
+      <c r="A6" s="118"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -30894,32 +30874,32 @@
       <c r="G6" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="121"/>
-      <c r="O6" s="121"/>
-      <c r="P6" s="121"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="I7" s="121"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="121"/>
-      <c r="L7" s="121"/>
-      <c r="M7" s="121"/>
-      <c r="N7" s="121"/>
-      <c r="O7" s="121"/>
-      <c r="P7" s="121"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="120" t="s">
+    <row r="8" spans="1:16">
+      <c r="A8" s="119" t="s">
         <v>116</v>
       </c>
       <c r="B8" s="50">
@@ -30945,17 +30925,17 @@
       <c r="G8" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
-      <c r="K8" s="121"/>
-      <c r="L8" s="121"/>
-      <c r="M8" s="121"/>
-      <c r="N8" s="121"/>
-      <c r="O8" s="121"/>
-      <c r="P8" s="121"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="120"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
+    <row r="9" spans="1:16">
+      <c r="A9" s="119"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -30979,17 +30959,17 @@
       <c r="G9" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="121"/>
-      <c r="J9" s="121"/>
-      <c r="K9" s="121"/>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="121"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="120"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
+    <row r="10" spans="1:16">
+      <c r="A10" s="119"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -31013,17 +30993,17 @@
       <c r="G10" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="121"/>
-      <c r="O10" s="121"/>
-      <c r="P10" s="121"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+      <c r="O10" s="120"/>
+      <c r="P10" s="120"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="120"/>
+    <row r="11" spans="1:16">
+      <c r="A11" s="119"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -31047,32 +31027,32 @@
       <c r="G11" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="I11" s="121"/>
-      <c r="J11" s="121"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="121"/>
-      <c r="M11" s="121"/>
-      <c r="N11" s="121"/>
-      <c r="O11" s="121"/>
-      <c r="P11" s="121"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="120"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
-      <c r="I12" s="121"/>
-      <c r="J12" s="121"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="121"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="121"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="121"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="119" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="118" t="s">
         <v>121</v>
       </c>
       <c r="B13" s="47">
@@ -31093,17 +31073,17 @@
       <c r="G13" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I13" s="121"/>
-      <c r="J13" s="121"/>
-      <c r="K13" s="121"/>
-      <c r="L13" s="121"/>
-      <c r="M13" s="121"/>
-      <c r="N13" s="121"/>
-      <c r="O13" s="121"/>
-      <c r="P13" s="121"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+      <c r="O13" s="120"/>
+      <c r="P13" s="120"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="119"/>
+    <row r="14" spans="1:16">
+      <c r="A14" s="118"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -31127,17 +31107,17 @@
       <c r="G14" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="I14" s="121"/>
-      <c r="J14" s="121"/>
-      <c r="K14" s="121"/>
-      <c r="L14" s="121"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="121"/>
-      <c r="O14" s="121"/>
-      <c r="P14" s="121"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="119"/>
+    <row r="15" spans="1:16">
+      <c r="A15" s="118"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -31161,17 +31141,17 @@
       <c r="G15" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="121"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="121"/>
-      <c r="L15" s="121"/>
-      <c r="M15" s="121"/>
-      <c r="N15" s="121"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="121"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="120"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="119"/>
+    <row r="16" spans="1:16">
+      <c r="A16" s="118"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -31195,17 +31175,17 @@
       <c r="G16" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="121"/>
-      <c r="J16" s="121"/>
-      <c r="K16" s="121"/>
-      <c r="L16" s="121"/>
-      <c r="M16" s="121"/>
-      <c r="N16" s="121"/>
-      <c r="O16" s="121"/>
-      <c r="P16" s="121"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="119" t="s">
+    <row r="17" spans="1:16">
+      <c r="A17" s="118" t="s">
         <v>125</v>
       </c>
       <c r="B17" s="50">
@@ -31231,17 +31211,17 @@
       <c r="G17" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
-      <c r="K17" s="121"/>
-      <c r="L17" s="121"/>
-      <c r="M17" s="121"/>
-      <c r="N17" s="121"/>
-      <c r="O17" s="121"/>
-      <c r="P17" s="121"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+      <c r="O17" s="120"/>
+      <c r="P17" s="120"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="119"/>
+    <row r="18" spans="1:16">
+      <c r="A18" s="118"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -31265,16 +31245,16 @@
       <c r="G18" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="I18" s="121"/>
-      <c r="J18" s="121"/>
-      <c r="K18" s="121"/>
-      <c r="L18" s="121"/>
-      <c r="M18" s="121"/>
-      <c r="N18" s="121"/>
-      <c r="O18" s="121"/>
-      <c r="P18" s="121"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+      <c r="O18" s="120"/>
+      <c r="P18" s="120"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="B19" t="s">
         <v>128</v>
       </c>
@@ -31291,22 +31271,22 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="54" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="55" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="56" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -31314,7 +31294,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="B25" s="57" t="s">
         <v>136</v>
       </c>
@@ -31337,14 +31317,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="F2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -31412,7 +31392,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -31451,7 +31431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -31488,7 +31468,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="48" customHeight="1">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -31525,7 +31505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="48" customHeight="1">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -31552,7 +31532,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="48" customHeight="1">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -31576,7 +31556,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="48" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>69</v>
@@ -31598,7 +31578,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -31633,7 +31613,7 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I2C development started, GPIO motor direction selct updated
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
@@ -32,12 +32,12 @@
     <definedName name="V_in" localSheetId="4">'Light sensor #2'!$B$5</definedName>
     <definedName name="V_in">'Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="301">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1239,15 +1239,51 @@
   <si>
     <t>0 - Go Forward / 1 - Go Backward</t>
   </si>
+  <si>
+    <t>I2C0SCL</t>
+  </si>
+  <si>
+    <t>I2C0SDA</t>
+  </si>
+  <si>
+    <t>Output - Clock</t>
+  </si>
+  <si>
+    <t>I2C module 0 data.</t>
+  </si>
+  <si>
+    <t>I2C module 0 clock.</t>
+  </si>
+  <si>
+    <t>Accelerometer I2C clock</t>
+  </si>
+  <si>
+    <t>Accelerometer I2C data</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>High = I2C, Low = SPI</t>
+  </si>
+  <si>
+    <t>Accelerometer chip select</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2641,7 +2677,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>483179</xdr:colOff>
+      <xdr:colOff>483180</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>96308</xdr:rowOff>
     </xdr:to>
@@ -6888,7 +6924,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6920,9 +6956,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6954,6 +6991,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7129,14 +7167,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
@@ -7144,7 +7182,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="61"/>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -7162,7 +7200,7 @@
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="61"/>
       <c r="B2" s="60" t="s">
         <v>160</v>
@@ -7186,10 +7224,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="61"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
         <v>194</v>
       </c>
@@ -7200,7 +7238,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
         <v>194</v>
       </c>
@@ -7214,7 +7252,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="61"/>
       <c r="B6" s="1" t="s">
         <v>157</v>
@@ -7223,7 +7261,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>
       <c r="B7" s="1" t="s">
         <v>157</v>
@@ -7232,7 +7270,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="61"/>
       <c r="B8" s="1" t="s">
         <v>157</v>
@@ -7241,10 +7279,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="61"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="61"/>
       <c r="B10" s="1" t="s">
         <v>144</v>
@@ -7253,7 +7291,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="61"/>
       <c r="B11" s="1" t="s">
         <v>144</v>
@@ -7262,7 +7300,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>195</v>
       </c>
@@ -7273,7 +7311,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="61" t="s">
         <v>195</v>
       </c>
@@ -7284,7 +7322,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
         <v>195</v>
       </c>
@@ -7295,7 +7333,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
         <v>195</v>
       </c>
@@ -7306,7 +7344,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="61"/>
       <c r="B16" s="1" t="s">
         <v>144</v>
@@ -7315,7 +7353,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="61"/>
       <c r="B17" s="1" t="s">
         <v>144</v>
@@ -7324,7 +7362,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
         <v>195</v>
       </c>
@@ -7335,7 +7373,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="61"/>
       <c r="B19" s="1" t="s">
         <v>147</v>
@@ -7344,10 +7382,10 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="61"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
         <v>195</v>
       </c>
@@ -7358,7 +7396,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="61"/>
       <c r="B22" s="1" t="s">
         <v>154</v>
@@ -7367,7 +7405,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="61"/>
       <c r="B23" s="46" t="s">
         <v>154</v>
@@ -7376,47 +7414,47 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="61"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="61"/>
       <c r="B25" s="86"/>
       <c r="C25" s="86" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="61"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="61"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="61"/>
     </row>
   </sheetData>
@@ -7426,14 +7464,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -7501,7 +7539,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -7590,7 +7628,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7680,7 +7718,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -7770,7 +7808,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -7894,7 +7932,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -8020,7 +8058,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -8138,7 +8176,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -8252,7 +8290,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -8364,7 +8402,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -8478,7 +8516,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -8590,7 +8628,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -8704,7 +8742,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -8864,7 +8902,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -9030,7 +9068,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -9194,7 +9232,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -9348,7 +9386,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -9502,7 +9540,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -9666,7 +9704,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -9834,7 +9872,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -10004,7 +10042,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -10156,7 +10194,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -10286,7 +10324,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -10402,7 +10440,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -10526,7 +10564,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -10650,7 +10688,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -10772,7 +10810,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -10892,7 +10930,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -11010,7 +11048,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -11124,7 +11162,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -11238,7 +11276,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -11348,7 +11386,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -11458,7 +11496,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -11568,7 +11606,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -11678,7 +11716,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -11788,7 +11826,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -11900,7 +11938,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -12014,7 +12052,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -12124,7 +12162,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -12234,7 +12272,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12341,7 +12379,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -12439,7 +12477,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -12528,7 +12566,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -12617,7 +12655,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -12706,7 +12744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -12792,7 +12830,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -12878,7 +12916,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -12964,7 +13002,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -13050,7 +13088,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -13136,7 +13174,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -13474,7 +13512,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -13812,7 +13850,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -14150,7 +14188,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -14488,7 +14526,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -14826,7 +14864,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -15176,14 +15214,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -15252,7 +15290,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15425,7 +15463,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -15599,7 +15637,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -15829,7 +15867,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -16031,7 +16069,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -16233,7 +16271,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -16447,7 +16485,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -16663,7 +16701,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -16875,7 +16913,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -17087,7 +17125,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -17313,7 +17351,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -17487,7 +17525,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -17673,7 +17711,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -17871,7 +17909,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -18065,7 +18103,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -18251,7 +18289,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -18443,7 +18481,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -18637,7 +18675,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -18831,7 +18869,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -19013,7 +19051,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -19195,7 +19233,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -19389,7 +19427,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -19577,7 +19615,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -19771,7 +19809,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -19953,7 +19991,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -20137,7 +20175,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -20363,7 +20401,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -20545,7 +20583,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -20727,7 +20765,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -20927,7 +20965,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -21145,7 +21183,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -21333,7 +21371,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -21525,7 +21563,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -21717,7 +21755,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -21907,7 +21945,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -22097,7 +22135,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -22289,7 +22327,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -22481,7 +22519,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -22673,7 +22711,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -22866,7 +22904,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -23090,7 +23128,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -23285,7 +23323,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -23518,7 +23556,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -23741,7 +23779,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -23943,7 +23981,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -24225,7 +24263,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -24403,7 +24441,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -24605,7 +24643,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -24777,7 +24815,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -25115,7 +25153,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -25453,7 +25491,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -25791,7 +25829,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -26129,7 +26167,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -26467,7 +26505,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -27112,14 +27150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="62" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="62" customWidth="1"/>
@@ -27135,7 +27173,7 @@
     <col min="40" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="65"/>
@@ -27172,7 +27210,7 @@
       <c r="AL1" s="65"/>
       <c r="AM1" s="65"/>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="64"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66">
@@ -27221,7 +27259,7 @@
       <c r="AL2" s="66"/>
       <c r="AM2" s="65"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="64"/>
       <c r="B3" s="66">
         <v>1</v>
@@ -27280,7 +27318,7 @@
       <c r="AL3" s="66"/>
       <c r="AM3" s="65"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="64"/>
       <c r="B4" s="66"/>
       <c r="C4" s="66">
@@ -27341,7 +27379,7 @@
       <c r="AL4" s="66"/>
       <c r="AM4" s="65"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="66">
         <v>1</v>
@@ -27406,7 +27444,7 @@
       </c>
       <c r="AM5" s="65"/>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66">
@@ -27471,7 +27509,7 @@
       </c>
       <c r="AM6" s="65"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="66">
         <v>1</v>
@@ -27538,7 +27576,7 @@
       <c r="AL7" s="66"/>
       <c r="AM7" s="65"/>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="64"/>
       <c r="B8" s="66"/>
       <c r="C8" s="66">
@@ -27599,7 +27637,7 @@
       <c r="AL8" s="66"/>
       <c r="AM8" s="64"/>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="64"/>
       <c r="B9" s="66">
         <v>1</v>
@@ -27660,7 +27698,7 @@
       <c r="AL9" s="66"/>
       <c r="AM9" s="64"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -27697,7 +27735,7 @@
       <c r="AL10" s="64"/>
       <c r="AM10" s="64"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12" s="63" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -27799,7 +27837,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="64"/>
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
@@ -27836,7 +27874,7 @@
       <c r="AL14" s="65"/>
       <c r="AM14" s="65"/>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="64"/>
       <c r="B15" s="66"/>
       <c r="C15" s="66"/>
@@ -27879,7 +27917,7 @@
       <c r="AL15" s="66"/>
       <c r="AM15" s="65"/>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="64"/>
       <c r="B16" s="66"/>
       <c r="C16" s="66"/>
@@ -27932,7 +27970,7 @@
       <c r="AL16" s="66"/>
       <c r="AM16" s="65"/>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="64"/>
       <c r="B17" s="66">
         <v>1</v>
@@ -28005,7 +28043,7 @@
       </c>
       <c r="AM17" s="65"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="64"/>
       <c r="B18" s="66"/>
       <c r="C18" s="66">
@@ -28068,7 +28106,7 @@
       </c>
       <c r="AM18" s="65"/>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="64"/>
       <c r="B19" s="66"/>
       <c r="C19" s="66"/>
@@ -28119,7 +28157,7 @@
       </c>
       <c r="AM19" s="65"/>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="64"/>
       <c r="B20" s="66"/>
       <c r="C20" s="66"/>
@@ -28172,7 +28210,7 @@
       </c>
       <c r="AM20" s="65"/>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
       <c r="B21" s="66"/>
       <c r="C21" s="66">
@@ -28231,7 +28269,7 @@
       <c r="AL21" s="66"/>
       <c r="AM21" s="64"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="64"/>
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
@@ -28274,7 +28312,7 @@
       <c r="AL22" s="66"/>
       <c r="AM22" s="64"/>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="64"/>
       <c r="B23" s="64"/>
       <c r="C23" s="64"/>
@@ -28311,7 +28349,7 @@
       <c r="AL23" s="64"/>
       <c r="AM23" s="64"/>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B25" s="63" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -28499,21 +28537,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>166</v>
       </c>
@@ -28521,7 +28559,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -28535,7 +28573,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -28549,7 +28587,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>1</v>
       </c>
@@ -28560,7 +28598,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>167</v>
       </c>
@@ -28574,7 +28612,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L6">
         <v>2</v>
       </c>
@@ -28585,7 +28623,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L7">
         <v>3</v>
       </c>
@@ -28596,22 +28634,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L11">
         <v>7</v>
       </c>
@@ -28629,17 +28667,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.140625" bestFit="1" customWidth="1"/>
@@ -28647,7 +28685,7 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -28670,7 +28708,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>33</v>
       </c>
@@ -28684,7 +28722,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="103"/>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -28696,13 +28734,13 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="103"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>291</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>42</v>
@@ -28718,7 +28756,7 @@
       </c>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="103"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
@@ -28740,7 +28778,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="103"/>
       <c r="B6" s="1" t="s">
         <v>38</v>
@@ -28754,7 +28792,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="103"/>
       <c r="B7" s="1" t="s">
         <v>39</v>
@@ -28776,7 +28814,7 @@
       </c>
       <c r="H7" s="59"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="103"/>
       <c r="B8" s="1" t="s">
         <v>40</v>
@@ -28798,7 +28836,7 @@
       </c>
       <c r="H8" s="58"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="103"/>
       <c r="B9" s="1" t="s">
         <v>41</v>
@@ -28820,7 +28858,7 @@
       </c>
       <c r="H9" s="101"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="103" t="s">
         <v>276</v>
       </c>
@@ -28834,7 +28872,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="103"/>
       <c r="B12" s="1" t="s">
         <v>278</v>
@@ -28846,31 +28884,51 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="103"/>
       <c r="B13" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="103"/>
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="C14" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H14" s="59"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="103"/>
       <c r="B15" s="1" t="s">
         <v>281</v>
@@ -28882,7 +28940,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="103"/>
       <c r="B16" s="1" t="s">
         <v>282</v>
@@ -28894,7 +28952,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="103"/>
       <c r="B17" s="1" t="s">
         <v>283</v>
@@ -28906,7 +28964,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="103" t="s">
         <v>27</v>
       </c>
@@ -28920,7 +28978,7 @@
       <c r="G19" s="102"/>
       <c r="H19" s="102"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="103"/>
       <c r="B20" s="102"/>
       <c r="C20" s="102"/>
@@ -28930,7 +28988,7 @@
       <c r="G20" s="102"/>
       <c r="H20" s="102"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="103"/>
       <c r="B21" s="102"/>
       <c r="C21" s="102"/>
@@ -28940,7 +28998,7 @@
       <c r="G21" s="102"/>
       <c r="H21" s="102"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="103"/>
       <c r="B22" s="102"/>
       <c r="C22" s="102"/>
@@ -28950,7 +29008,7 @@
       <c r="G22" s="102"/>
       <c r="H22" s="102"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="103"/>
       <c r="B23" s="99" t="s">
         <v>208</v>
@@ -28966,7 +29024,7 @@
       <c r="G23" s="99"/>
       <c r="H23" s="99"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="103"/>
       <c r="B24" s="99" t="s">
         <v>209</v>
@@ -28984,7 +29042,7 @@
       <c r="G24" s="99"/>
       <c r="H24" s="99"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="103"/>
       <c r="B25" s="99" t="s">
         <v>28</v>
@@ -29002,7 +29060,7 @@
       <c r="G25" s="99"/>
       <c r="H25" s="99"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="103"/>
       <c r="B26" s="99" t="s">
         <v>29</v>
@@ -29022,7 +29080,7 @@
       <c r="G26" s="99"/>
       <c r="H26" s="99"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="103" t="s">
         <v>25</v>
       </c>
@@ -29040,7 +29098,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="103"/>
       <c r="B29" s="1" t="s">
         <v>22</v>
@@ -29056,7 +29114,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="103"/>
       <c r="B30" s="100" t="s">
         <v>268</v>
@@ -29078,7 +29136,7 @@
       </c>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="103"/>
       <c r="B31" s="1" t="s">
         <v>253</v>
@@ -29100,21 +29158,31 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="103" t="s">
         <v>257</v>
       </c>
       <c r="B33" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="103"/>
       <c r="B34" s="1" t="s">
         <v>259</v>
@@ -29136,7 +29204,7 @@
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="103"/>
       <c r="B35" s="1" t="s">
         <v>260</v>
@@ -29158,7 +29226,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="103"/>
       <c r="B36" s="1" t="s">
         <v>261</v>
@@ -29180,7 +29248,7 @@
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="103" t="s">
         <v>26</v>
       </c>
@@ -29202,7 +29270,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="103"/>
       <c r="B39" s="2" t="s">
         <v>11</v>
@@ -29222,7 +29290,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="103"/>
       <c r="B40" s="3" t="s">
         <v>9</v>
@@ -29244,7 +29312,7 @@
       </c>
       <c r="H40" s="98"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="103"/>
       <c r="B41" s="4" t="s">
         <v>10</v>
@@ -29266,7 +29334,7 @@
       </c>
       <c r="H41" s="72"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="103"/>
       <c r="B42" s="1" t="s">
         <v>3</v>
@@ -29286,7 +29354,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>16</v>
       </c>
@@ -29297,7 +29365,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>18</v>
       </c>
@@ -29322,14 +29390,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29338,7 +29406,7 @@
     <col min="12" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -29370,7 +29438,7 @@
       </c>
       <c r="M1" s="109"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -29402,7 +29470,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>216</v>
       </c>
@@ -29435,7 +29503,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>217</v>
       </c>
@@ -29476,7 +29544,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -29509,7 +29577,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -29536,7 +29604,7 @@
       </c>
       <c r="Q6" s="85"/>
     </row>
-    <row r="7" spans="1:17" ht="18">
+    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -29572,7 +29640,7 @@
       </c>
       <c r="Q7" s="86"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -29594,7 +29662,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -29625,7 +29693,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -29656,7 +29724,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -29699,14 +29767,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29715,7 +29783,7 @@
     <col min="12" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -29751,7 +29819,7 @@
       </c>
       <c r="O1" s="109"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -29789,7 +29857,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>247</v>
       </c>
@@ -29824,7 +29892,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>248</v>
       </c>
@@ -29873,7 +29941,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18">
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -29914,7 +29982,7 @@
         <v>9.6116504854368928E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -29949,7 +30017,7 @@
       </c>
       <c r="U6" s="85"/>
     </row>
-    <row r="7" spans="1:21" ht="18">
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -29993,7 +30061,7 @@
       </c>
       <c r="U7" s="86"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -30023,7 +30091,7 @@
         <v>2.9117647058823528</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -30062,7 +30130,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -30101,7 +30169,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -30131,7 +30199,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L12" s="97" t="s">
         <v>252</v>
       </c>
@@ -30139,7 +30207,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N13" s="96" t="s">
         <v>252</v>
       </c>
@@ -30169,26 +30237,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>164</v>
       </c>
@@ -30200,14 +30268,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -30219,7 +30287,7 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>99</v>
       </c>
@@ -30254,7 +30322,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>98</v>
       </c>
@@ -30295,7 +30363,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>94</v>
       </c>
@@ -30336,7 +30404,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>87</v>
       </c>
@@ -30377,13 +30445,13 @@
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>80</v>
       </c>
@@ -30399,7 +30467,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>78</v>
       </c>
@@ -30416,7 +30484,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>170</v>
       </c>
@@ -30424,22 +30492,22 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -30460,7 +30528,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -30478,7 +30546,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>165</v>
       </c>
@@ -30490,14 +30558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -30506,7 +30574,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
@@ -30526,7 +30594,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -30550,7 +30618,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>107</v>
       </c>
@@ -30578,14 +30646,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="113" t="s">
         <v>108</v>
       </c>
@@ -30618,7 +30686,7 @@
       <c r="O5" s="115"/>
       <c r="P5" s="115"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="113"/>
       <c r="B6" s="50">
         <f>B5/60</f>
@@ -30652,7 +30720,7 @@
       <c r="O6" s="115"/>
       <c r="P6" s="115"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -30667,7 +30735,7 @@
       <c r="O7" s="115"/>
       <c r="P7" s="115"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="114" t="s">
         <v>111</v>
       </c>
@@ -30703,7 +30771,7 @@
       <c r="O8" s="115"/>
       <c r="P8" s="115"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="114"/>
       <c r="B9" s="50">
         <f>B8/10</f>
@@ -30737,7 +30805,7 @@
       <c r="O9" s="115"/>
       <c r="P9" s="115"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="114"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
@@ -30771,7 +30839,7 @@
       <c r="O10" s="115"/>
       <c r="P10" s="115"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="114"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
@@ -30805,7 +30873,7 @@
       <c r="O11" s="115"/>
       <c r="P11" s="115"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
@@ -30820,7 +30888,7 @@
       <c r="O12" s="115"/>
       <c r="P12" s="115"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="113" t="s">
         <v>116</v>
       </c>
@@ -30851,7 +30919,7 @@
       <c r="O13" s="115"/>
       <c r="P13" s="115"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="113"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
@@ -30885,7 +30953,7 @@
       <c r="O14" s="115"/>
       <c r="P14" s="115"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="113"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
@@ -30919,7 +30987,7 @@
       <c r="O15" s="115"/>
       <c r="P15" s="115"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="113"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
@@ -30953,7 +31021,7 @@
       <c r="O16" s="115"/>
       <c r="P16" s="115"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="113" t="s">
         <v>120</v>
       </c>
@@ -30989,7 +31057,7 @@
       <c r="O17" s="115"/>
       <c r="P17" s="115"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="113"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
@@ -31023,7 +31091,7 @@
       <c r="O18" s="115"/>
       <c r="P18" s="115"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -31040,22 +31108,22 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -31063,7 +31131,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>131</v>
       </c>
@@ -31086,14 +31154,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="F2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -31161,7 +31229,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -31200,7 +31268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -31237,7 +31305,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1">
+    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -31274,7 +31342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1">
+    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -31301,7 +31369,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1">
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -31325,7 +31393,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1">
+    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>64</v>
@@ -31347,7 +31415,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -31382,7 +31450,7 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
I2C Service development - WIP
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="838" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do!!!" sheetId="10" r:id="rId1"/>
@@ -7235,7 +7235,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29037,8 +29037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30928,7 +30928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SSI and Shift register handler development
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="309">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1279,6 +1279,27 @@
   <si>
     <t>http://playground.arduino.cc/Main/MMA7455</t>
   </si>
+  <si>
+    <t>PD2</t>
+  </si>
+  <si>
+    <t>PD3</t>
+  </si>
+  <si>
+    <t>SSI3Clk</t>
+  </si>
+  <si>
+    <t>SSI3Rx</t>
+  </si>
+  <si>
+    <t>SSI3Tx</t>
+  </si>
+  <si>
+    <t>serial data</t>
+  </si>
+  <si>
+    <t>SSI3Fss - slave select</t>
+  </si>
 </sst>
 </file>
 
@@ -1887,7 +1908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2106,6 +2127,8 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -29035,10 +29058,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29451,86 +29474,110 @@
       <c r="A28" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="D28" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="116"/>
+      <c r="F28" s="117" t="s">
+        <v>304</v>
+      </c>
+      <c r="G28" s="116" t="s">
+        <v>151</v>
+      </c>
+      <c r="H28" s="116"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="103"/>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="D29" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="116"/>
+      <c r="F29" s="117" t="s">
+        <v>308</v>
+      </c>
+      <c r="G29" s="116" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="116"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="103"/>
-      <c r="B30" s="100" t="s">
-        <v>268</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F30" s="70" t="s">
-        <v>288</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="H30" s="3"/>
+      <c r="B30" s="116" t="s">
+        <v>302</v>
+      </c>
+      <c r="C30" s="116" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116" t="s">
+        <v>305</v>
+      </c>
+      <c r="G30" s="116" t="s">
+        <v>307</v>
+      </c>
+      <c r="H30" s="116"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="103"/>
-      <c r="B31" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="116" t="s">
+        <v>303</v>
+      </c>
+      <c r="C31" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="116" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="116"/>
+      <c r="F31" s="117" t="s">
+        <v>306</v>
+      </c>
+      <c r="G31" s="116" t="s">
+        <v>307</v>
+      </c>
+      <c r="H31" s="116"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="103"/>
+      <c r="B32" s="100" t="s">
+        <v>268</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F31" s="70" t="s">
+      <c r="E32" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F32" s="70" t="s">
         <v>288</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H31" s="4"/>
+      <c r="G32" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="103" t="s">
-        <v>257</v>
-      </c>
-      <c r="B33" s="100" t="s">
-        <v>258</v>
+      <c r="A33" s="103"/>
+      <c r="B33" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -29539,215 +29586,239 @@
         <v>204</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>299</v>
+        <v>285</v>
+      </c>
+      <c r="F33" s="70" t="s">
+        <v>288</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="103"/>
-      <c r="B34" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C34" s="74" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="103"/>
-      <c r="B35" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C35" s="74" t="s">
-        <v>6</v>
+      <c r="A35" s="103" t="s">
+        <v>257</v>
+      </c>
+      <c r="B35" s="100" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>264</v>
+        <v>204</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="1"/>
+        <v>298</v>
+      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="103"/>
       <c r="B36" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C36" s="74" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="103" t="s">
-        <v>26</v>
-      </c>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="103"/>
+      <c r="B37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="103"/>
       <c r="B38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" s="74" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>207</v>
+        <v>262</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" s="70" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="1"/>
+        <v>267</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="103"/>
-      <c r="B39" s="2" t="s">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="103" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="103"/>
+      <c r="B41" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F39" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="103"/>
-      <c r="B40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F40" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H40" s="98"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="103"/>
-      <c r="B41" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>287</v>
+        <v>137</v>
       </c>
       <c r="F41" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H41" s="72"/>
+        <v>138</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="103"/>
-      <c r="B42" s="1" t="s">
-        <v>3</v>
+      <c r="B42" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>207</v>
+        <v>141</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
       <c r="F42" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H42" s="98"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="103"/>
+      <c r="B43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F43" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="A44" s="103"/>
+      <c r="B44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>16</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>17</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>18</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B19:H22"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="A40:A44"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A35:A38"/>
     <mergeCell ref="A11:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
started inplementing ssOS to Droidbot SW
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="930" activeTab="2"/>
@@ -33,12 +33,12 @@
     <definedName name="V_in" localSheetId="5">'Light sensor #2'!$B$5</definedName>
     <definedName name="V_in">'Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="318">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1324,15 +1324,18 @@
   <si>
     <t>register. See Figure 9.</t>
   </si>
+  <si>
+    <t>Pull up, low level interrupt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1938,7 +1941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2117,6 +2120,8 @@
     <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2159,8 +2164,7 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2794,7 +2798,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2814,7 +2818,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -7090,7 +7094,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7122,9 +7126,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7156,6 +7161,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7331,14 +7337,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
@@ -7346,7 +7352,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="61"/>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -7364,7 +7370,7 @@
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="61"/>
       <c r="B2" s="60" t="s">
         <v>160</v>
@@ -7388,10 +7394,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="61"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
         <v>194</v>
       </c>
@@ -7402,7 +7408,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
         <v>194</v>
       </c>
@@ -7416,7 +7422,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="61"/>
       <c r="B6" s="1" t="s">
         <v>157</v>
@@ -7425,7 +7431,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="61"/>
       <c r="B7" s="1" t="s">
         <v>157</v>
@@ -7434,7 +7440,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="61"/>
       <c r="B8" s="1" t="s">
         <v>157</v>
@@ -7443,10 +7449,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="61"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="61"/>
       <c r="B10" s="1" t="s">
         <v>144</v>
@@ -7455,7 +7461,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="61"/>
       <c r="B11" s="1" t="s">
         <v>144</v>
@@ -7464,7 +7470,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="61" t="s">
         <v>195</v>
       </c>
@@ -7475,7 +7481,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="61" t="s">
         <v>195</v>
       </c>
@@ -7486,7 +7492,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
         <v>195</v>
       </c>
@@ -7497,7 +7503,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="61" t="s">
         <v>195</v>
       </c>
@@ -7508,7 +7514,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="61"/>
       <c r="B16" s="1" t="s">
         <v>144</v>
@@ -7517,7 +7523,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="61"/>
       <c r="B17" s="1" t="s">
         <v>144</v>
@@ -7526,7 +7532,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="61" t="s">
         <v>195</v>
       </c>
@@ -7537,7 +7543,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="61"/>
       <c r="B19" s="1" t="s">
         <v>147</v>
@@ -7546,10 +7552,10 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="61"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="61" t="s">
         <v>195</v>
       </c>
@@ -7560,7 +7566,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="61"/>
       <c r="B22" s="1" t="s">
         <v>154</v>
@@ -7569,7 +7575,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="61"/>
       <c r="B23" s="46" t="s">
         <v>154</v>
@@ -7578,47 +7584,47 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="61"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="61"/>
       <c r="B25" s="86"/>
       <c r="C25" s="86" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="61"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="61"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="61"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="61"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="61"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="61"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="61"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="61"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="61"/>
     </row>
   </sheetData>
@@ -7628,14 +7634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="F2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -7703,7 +7709,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -7742,7 +7748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -7779,7 +7785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1">
+    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -7816,7 +7822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1">
+    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -7843,7 +7849,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1">
+    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -7867,7 +7873,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1">
+    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>64</v>
@@ -7889,7 +7895,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -7924,21 +7930,21 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -8006,7 +8012,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -8095,7 +8101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8185,7 +8191,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -8275,7 +8281,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -8399,7 +8405,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -8525,7 +8531,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -8643,7 +8649,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -8757,7 +8763,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -8869,7 +8875,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -8983,7 +8989,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -9095,7 +9101,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -9209,7 +9215,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -9369,7 +9375,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -9535,7 +9541,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -9699,7 +9705,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -9853,7 +9859,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -10007,7 +10013,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -10171,7 +10177,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -10339,7 +10345,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -10509,7 +10515,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -10661,7 +10667,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -10791,7 +10797,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -10907,7 +10913,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -11031,7 +11037,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -11155,7 +11161,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -11277,7 +11283,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -11397,7 +11403,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -11515,7 +11521,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -11629,7 +11635,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -11743,7 +11749,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -11853,7 +11859,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -11963,7 +11969,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -12073,7 +12079,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -12183,7 +12189,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -12293,7 +12299,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -12405,7 +12411,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -12519,7 +12525,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -12629,7 +12635,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -12739,7 +12745,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12846,7 +12852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -12944,7 +12950,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -13033,7 +13039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -13122,7 +13128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -13211,7 +13217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -13297,7 +13303,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -13383,7 +13389,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -13469,7 +13475,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -13555,7 +13561,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -13641,7 +13647,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -13979,7 +13985,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -14317,7 +14323,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -14655,7 +14661,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -14993,7 +14999,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -15331,7 +15337,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -15681,14 +15687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -15757,7 +15763,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15930,7 +15936,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -16104,7 +16110,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -16334,7 +16340,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -16536,7 +16542,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -16738,7 +16744,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -16952,7 +16958,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -17168,7 +17174,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -17380,7 +17386,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -17592,7 +17598,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -17818,7 +17824,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -17992,7 +17998,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -18178,7 +18184,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -18376,7 +18382,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -18570,7 +18576,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -18756,7 +18762,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -18948,7 +18954,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -19142,7 +19148,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -19336,7 +19342,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -19518,7 +19524,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -19700,7 +19706,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -19894,7 +19900,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -20082,7 +20088,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -20276,7 +20282,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -20458,7 +20464,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -20642,7 +20648,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -20868,7 +20874,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -21050,7 +21056,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -21232,7 +21238,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -21432,7 +21438,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -21650,7 +21656,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -21838,7 +21844,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -22030,7 +22036,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -22222,7 +22228,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -22412,7 +22418,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -22602,7 +22608,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -22794,7 +22800,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -22986,7 +22992,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -23178,7 +23184,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -23371,7 +23377,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -23595,7 +23601,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -23790,7 +23796,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -24023,7 +24029,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -24246,7 +24252,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -24448,7 +24454,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -24730,7 +24736,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -24908,7 +24914,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -25110,7 +25116,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -25282,7 +25288,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84">
+    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -25620,7 +25626,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84">
+    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -25958,7 +25964,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84">
+    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -26296,7 +26302,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84">
+    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -26634,7 +26640,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84">
+    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -26972,7 +26978,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84">
+    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -27617,14 +27623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="62" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="62" customWidth="1"/>
@@ -27640,7 +27646,7 @@
     <col min="40" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="65"/>
@@ -27677,7 +27683,7 @@
       <c r="AL1" s="65"/>
       <c r="AM1" s="65"/>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="64"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66">
@@ -27726,7 +27732,7 @@
       <c r="AL2" s="66"/>
       <c r="AM2" s="65"/>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="64"/>
       <c r="B3" s="66">
         <v>1</v>
@@ -27785,7 +27791,7 @@
       <c r="AL3" s="66"/>
       <c r="AM3" s="65"/>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="64"/>
       <c r="B4" s="66"/>
       <c r="C4" s="66">
@@ -27846,7 +27852,7 @@
       <c r="AL4" s="66"/>
       <c r="AM4" s="65"/>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="66">
         <v>1</v>
@@ -27911,7 +27917,7 @@
       </c>
       <c r="AM5" s="65"/>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="64"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66">
@@ -27976,7 +27982,7 @@
       </c>
       <c r="AM6" s="65"/>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="64"/>
       <c r="B7" s="66">
         <v>1</v>
@@ -28043,7 +28049,7 @@
       <c r="AL7" s="66"/>
       <c r="AM7" s="65"/>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="64"/>
       <c r="B8" s="66"/>
       <c r="C8" s="66">
@@ -28104,7 +28110,7 @@
       <c r="AL8" s="66"/>
       <c r="AM8" s="64"/>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="64"/>
       <c r="B9" s="66">
         <v>1</v>
@@ -28165,7 +28171,7 @@
       <c r="AL9" s="66"/>
       <c r="AM9" s="64"/>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -28202,7 +28208,7 @@
       <c r="AL10" s="64"/>
       <c r="AM10" s="64"/>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B12" s="63" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -28304,7 +28310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="64"/>
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
@@ -28341,7 +28347,7 @@
       <c r="AL14" s="65"/>
       <c r="AM14" s="65"/>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="64"/>
       <c r="B15" s="66"/>
       <c r="C15" s="66"/>
@@ -28384,7 +28390,7 @@
       <c r="AL15" s="66"/>
       <c r="AM15" s="65"/>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="64"/>
       <c r="B16" s="66"/>
       <c r="C16" s="66"/>
@@ -28437,7 +28443,7 @@
       <c r="AL16" s="66"/>
       <c r="AM16" s="65"/>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="64"/>
       <c r="B17" s="66">
         <v>1</v>
@@ -28510,7 +28516,7 @@
       </c>
       <c r="AM17" s="65"/>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="64"/>
       <c r="B18" s="66"/>
       <c r="C18" s="66">
@@ -28573,7 +28579,7 @@
       </c>
       <c r="AM18" s="65"/>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="64"/>
       <c r="B19" s="66"/>
       <c r="C19" s="66"/>
@@ -28624,7 +28630,7 @@
       </c>
       <c r="AM19" s="65"/>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="64"/>
       <c r="B20" s="66"/>
       <c r="C20" s="66"/>
@@ -28677,7 +28683,7 @@
       </c>
       <c r="AM20" s="65"/>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
       <c r="B21" s="66"/>
       <c r="C21" s="66">
@@ -28736,7 +28742,7 @@
       <c r="AL21" s="66"/>
       <c r="AM21" s="64"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="64"/>
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
@@ -28779,7 +28785,7 @@
       <c r="AL22" s="66"/>
       <c r="AM22" s="64"/>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="64"/>
       <c r="B23" s="64"/>
       <c r="C23" s="64"/>
@@ -28816,7 +28822,7 @@
       <c r="AL23" s="64"/>
       <c r="AM23" s="64"/>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B25" s="63" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -29004,21 +29010,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>166</v>
       </c>
@@ -29026,7 +29032,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -29040,7 +29046,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -29054,7 +29060,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L4">
         <v>1</v>
       </c>
@@ -29065,7 +29071,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>167</v>
       </c>
@@ -29079,7 +29085,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L6">
         <v>2</v>
       </c>
@@ -29090,7 +29096,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L7">
         <v>3</v>
       </c>
@@ -29101,22 +29107,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L11">
         <v>7</v>
       </c>
@@ -29134,14 +29140,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -29152,7 +29158,7 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -29175,8 +29181,8 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="105" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="107" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -29189,8 +29195,8 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="105"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="107"/>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
@@ -29201,8 +29207,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="105"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -29223,8 +29229,8 @@
       </c>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="105"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -29245,8 +29251,8 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="105"/>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="107"/>
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
@@ -29259,8 +29265,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="105"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="107"/>
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
@@ -29281,8 +29287,8 @@
       </c>
       <c r="H7" s="59"/>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="105"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
@@ -29303,8 +29309,8 @@
       </c>
       <c r="H8" s="58"/>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="105"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
@@ -29325,8 +29331,8 @@
       </c>
       <c r="H9" s="101"/>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="105" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="107" t="s">
         <v>276</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -29339,8 +29345,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="105"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="107"/>
       <c r="B12" s="1" t="s">
         <v>278</v>
       </c>
@@ -29351,8 +29357,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="105"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
       <c r="B13" s="1" t="s">
         <v>279</v>
       </c>
@@ -29371,10 +29377,10 @@
       <c r="G13" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H13" s="118"/>
+      <c r="H13" s="104"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="105"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="107"/>
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -29393,10 +29399,10 @@
       <c r="G14" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="H14" s="119"/>
+      <c r="H14" s="105"/>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="105"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="107"/>
       <c r="B15" s="1" t="s">
         <v>281</v>
       </c>
@@ -29407,8 +29413,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="105"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="107"/>
       <c r="B16" s="1" t="s">
         <v>282</v>
       </c>
@@ -29419,8 +29425,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="105"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="107"/>
       <c r="B17" s="1" t="s">
         <v>283</v>
       </c>
@@ -29431,52 +29437,52 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="105" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="106" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="104"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="104"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="105"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="104"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="107"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="105"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="107"/>
+      <c r="B21" s="106"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="105"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="104"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="107"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="106"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="106"/>
+      <c r="H22" s="106"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="105"/>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="107"/>
       <c r="B23" s="99" t="s">
         <v>208</v>
       </c>
@@ -29491,8 +29497,8 @@
       <c r="G23" s="99"/>
       <c r="H23" s="99"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="105"/>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="107"/>
       <c r="B24" s="99" t="s">
         <v>209</v>
       </c>
@@ -29509,8 +29515,8 @@
       <c r="G24" s="99"/>
       <c r="H24" s="99"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="105"/>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="107"/>
       <c r="B25" s="99" t="s">
         <v>28</v>
       </c>
@@ -29527,8 +29533,8 @@
       <c r="G25" s="99"/>
       <c r="H25" s="99"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="105"/>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="107"/>
       <c r="B26" s="99" t="s">
         <v>29</v>
       </c>
@@ -29547,8 +29553,8 @@
       <c r="G26" s="99"/>
       <c r="H26" s="99"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="105" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="107" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="102" t="s">
@@ -29569,8 +29575,8 @@
       </c>
       <c r="H28" s="102"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="105"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="107"/>
       <c r="B29" s="102" t="s">
         <v>22</v>
       </c>
@@ -29589,8 +29595,8 @@
       </c>
       <c r="H29" s="102"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="105"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="107"/>
       <c r="B30" s="102" t="s">
         <v>302</v>
       </c>
@@ -29609,8 +29615,8 @@
       </c>
       <c r="H30" s="102"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="105"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="107"/>
       <c r="B31" s="102" t="s">
         <v>303</v>
       </c>
@@ -29629,8 +29635,8 @@
       </c>
       <c r="H31" s="102"/>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="105"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="107"/>
       <c r="B32" s="100" t="s">
         <v>268</v>
       </c>
@@ -29651,8 +29657,8 @@
       </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="105"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="107"/>
       <c r="B33" s="1" t="s">
         <v>253</v>
       </c>
@@ -29673,8 +29679,8 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="105" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="107" t="s">
         <v>257</v>
       </c>
       <c r="B35" s="100" t="s">
@@ -29697,8 +29703,8 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="105"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="107"/>
       <c r="B36" s="1" t="s">
         <v>259</v>
       </c>
@@ -29719,8 +29725,8 @@
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="105"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="107"/>
       <c r="B37" s="1" t="s">
         <v>260</v>
       </c>
@@ -29741,8 +29747,8 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="105"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="107"/>
       <c r="B38" s="1" t="s">
         <v>261</v>
       </c>
@@ -29763,8 +29769,8 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1">
-      <c r="A40" s="105" t="s">
+    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="107" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -29784,9 +29790,12 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
+      <c r="I40" s="120" t="s">
+        <v>317</v>
+      </c>
     </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
-      <c r="A41" s="105"/>
+    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="107"/>
       <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
@@ -29805,8 +29814,8 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="105"/>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="107"/>
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
@@ -29827,8 +29836,8 @@
       </c>
       <c r="H42" s="98"/>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="105"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="107"/>
       <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
@@ -29849,8 +29858,8 @@
       </c>
       <c r="H43" s="72"/>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="105"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="107"/>
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
@@ -29868,8 +29877,11 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
+      <c r="I44" s="120" t="s">
+        <v>317</v>
+      </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>16</v>
       </c>
@@ -29880,7 +29892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>18</v>
       </c>
@@ -29905,56 +29917,56 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P45"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="16:16">
+    <row r="2" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P2" s="57" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>316</v>
       </c>
@@ -29969,14 +29981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29985,7 +29997,7 @@
     <col min="12" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -30002,22 +30014,22 @@
       <c r="E1" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="111" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="106" t="s">
+      <c r="J1" s="115"/>
+      <c r="K1" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="111" t="s">
+      <c r="L1" s="113" t="s">
         <v>241</v>
       </c>
-      <c r="M1" s="111"/>
+      <c r="M1" s="113"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -30034,14 +30046,14 @@
       <c r="E2" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="110"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="80" t="s">
         <v>237</v>
       </c>
       <c r="J2" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="107"/>
+      <c r="K2" s="109"/>
       <c r="L2" s="80" t="s">
         <v>237</v>
       </c>
@@ -30049,7 +30061,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>216</v>
       </c>
@@ -30069,20 +30081,20 @@
       <c r="H3" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="112" t="s">
+      <c r="J3" s="115"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="114" t="s">
         <v>219</v>
       </c>
-      <c r="M3" s="113"/>
+      <c r="M3" s="115"/>
       <c r="P3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>217</v>
       </c>
@@ -30123,7 +30135,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18">
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -30156,7 +30168,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -30183,7 +30195,7 @@
       </c>
       <c r="Q6" s="85"/>
     </row>
-    <row r="7" spans="1:17" ht="18">
+    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -30219,7 +30231,7 @@
       </c>
       <c r="Q7" s="86"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -30241,7 +30253,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -30272,7 +30284,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -30303,7 +30315,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -30346,14 +30358,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -30362,7 +30374,7 @@
     <col min="12" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -30379,26 +30391,26 @@
       <c r="E1" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="109" t="s">
+      <c r="H1" s="111" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="114" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="106" t="s">
+      <c r="J1" s="115"/>
+      <c r="K1" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="111" t="s">
+      <c r="L1" s="113" t="s">
         <v>251</v>
       </c>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111" t="s">
+      <c r="M1" s="113"/>
+      <c r="N1" s="113" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="111"/>
+      <c r="O1" s="113"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -30415,14 +30427,14 @@
       <c r="E2" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="110"/>
+      <c r="H2" s="112"/>
       <c r="I2" s="80" t="s">
         <v>237</v>
       </c>
       <c r="J2" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="107"/>
+      <c r="K2" s="109"/>
       <c r="L2" s="80" t="s">
         <v>244</v>
       </c>
@@ -30436,7 +30448,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>247</v>
       </c>
@@ -30456,22 +30468,22 @@
       <c r="H3" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="I3" s="112" t="s">
+      <c r="I3" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="J3" s="113"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="112" t="s">
+      <c r="J3" s="115"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="114" t="s">
         <v>219</v>
       </c>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="113"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="115"/>
       <c r="T3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>248</v>
       </c>
@@ -30520,7 +30532,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18">
+    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -30561,7 +30573,7 @@
         <v>9.6116504854368928E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -30596,7 +30608,7 @@
       </c>
       <c r="U6" s="85"/>
     </row>
-    <row r="7" spans="1:21" ht="18">
+    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -30640,7 +30652,7 @@
       </c>
       <c r="U7" s="86"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -30670,7 +30682,7 @@
         <v>2.9117647058823528</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -30709,7 +30721,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -30748,7 +30760,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -30778,7 +30790,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="L12" s="97" t="s">
         <v>252</v>
       </c>
@@ -30786,7 +30798,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="N13" s="96" t="s">
         <v>252</v>
       </c>
@@ -30816,26 +30828,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>164</v>
       </c>
@@ -30847,14 +30859,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -30866,7 +30878,7 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>99</v>
       </c>
@@ -30901,7 +30913,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>98</v>
       </c>
@@ -30942,7 +30954,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>94</v>
       </c>
@@ -30983,7 +30995,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>87</v>
       </c>
@@ -31024,13 +31036,13 @@
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>80</v>
       </c>
@@ -31046,7 +31058,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>78</v>
       </c>
@@ -31063,7 +31075,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>170</v>
       </c>
@@ -31071,22 +31083,22 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -31107,7 +31119,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -31125,7 +31137,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>165</v>
       </c>
@@ -31137,14 +31149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -31153,7 +31165,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
@@ -31173,7 +31185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -31197,7 +31209,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
         <v>107</v>
       </c>
@@ -31225,15 +31237,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1">
-      <c r="A5" s="115" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="117" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="47">
@@ -31254,19 +31266,19 @@
       <c r="G5" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="117" t="s">
+      <c r="I5" s="119" t="s">
         <v>197</v>
       </c>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
-      <c r="N5" s="117"/>
-      <c r="O5" s="117"/>
-      <c r="P5" s="117"/>
+      <c r="J5" s="119"/>
+      <c r="K5" s="119"/>
+      <c r="L5" s="119"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="119"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="119"/>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="115"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="117"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -31290,32 +31302,32 @@
       <c r="G6" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="117"/>
-      <c r="J6" s="117"/>
-      <c r="K6" s="117"/>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
-      <c r="N6" s="117"/>
-      <c r="O6" s="117"/>
-      <c r="P6" s="117"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="119"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="117"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="119"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="119"/>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="116" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="118" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="50">
@@ -31341,17 +31353,17 @@
       <c r="G8" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="I8" s="117"/>
-      <c r="J8" s="117"/>
-      <c r="K8" s="117"/>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="117"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="117"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="119"/>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="116"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="118"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -31375,17 +31387,17 @@
       <c r="G9" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
-      <c r="N9" s="117"/>
-      <c r="O9" s="117"/>
-      <c r="P9" s="117"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="116"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="118"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -31409,17 +31421,17 @@
       <c r="G10" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="117"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
-      <c r="N10" s="117"/>
-      <c r="O10" s="117"/>
-      <c r="P10" s="117"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="119"/>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="116"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="118"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -31443,32 +31455,32 @@
       <c r="G11" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="117"/>
-      <c r="M11" s="117"/>
-      <c r="N11" s="117"/>
-      <c r="O11" s="117"/>
-      <c r="P11" s="117"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="119"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
-      <c r="I12" s="117"/>
-      <c r="J12" s="117"/>
-      <c r="K12" s="117"/>
-      <c r="L12" s="117"/>
-      <c r="M12" s="117"/>
-      <c r="N12" s="117"/>
-      <c r="O12" s="117"/>
-      <c r="P12" s="117"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="115" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="117" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="47">
@@ -31489,17 +31501,17 @@
       <c r="G13" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I13" s="117"/>
-      <c r="J13" s="117"/>
-      <c r="K13" s="117"/>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
-      <c r="O13" s="117"/>
-      <c r="P13" s="117"/>
+      <c r="I13" s="119"/>
+      <c r="J13" s="119"/>
+      <c r="K13" s="119"/>
+      <c r="L13" s="119"/>
+      <c r="M13" s="119"/>
+      <c r="N13" s="119"/>
+      <c r="O13" s="119"/>
+      <c r="P13" s="119"/>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="115"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="117"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -31523,17 +31535,17 @@
       <c r="G14" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="I14" s="117"/>
-      <c r="J14" s="117"/>
-      <c r="K14" s="117"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
+      <c r="I14" s="119"/>
+      <c r="J14" s="119"/>
+      <c r="K14" s="119"/>
+      <c r="L14" s="119"/>
+      <c r="M14" s="119"/>
+      <c r="N14" s="119"/>
+      <c r="O14" s="119"/>
+      <c r="P14" s="119"/>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="115"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="117"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -31557,17 +31569,17 @@
       <c r="G15" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="117"/>
-      <c r="J15" s="117"/>
-      <c r="K15" s="117"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-      <c r="N15" s="117"/>
-      <c r="O15" s="117"/>
-      <c r="P15" s="117"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="119"/>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="115"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="117"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -31591,17 +31603,17 @@
       <c r="G16" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="I16" s="117"/>
-      <c r="J16" s="117"/>
-      <c r="K16" s="117"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="117"/>
-      <c r="P16" s="117"/>
+      <c r="I16" s="119"/>
+      <c r="J16" s="119"/>
+      <c r="K16" s="119"/>
+      <c r="L16" s="119"/>
+      <c r="M16" s="119"/>
+      <c r="N16" s="119"/>
+      <c r="O16" s="119"/>
+      <c r="P16" s="119"/>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="115" t="s">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="117" t="s">
         <v>120</v>
       </c>
       <c r="B17" s="50">
@@ -31627,17 +31639,17 @@
       <c r="G17" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="I17" s="117"/>
-      <c r="J17" s="117"/>
-      <c r="K17" s="117"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-      <c r="N17" s="117"/>
-      <c r="O17" s="117"/>
-      <c r="P17" s="117"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="119"/>
+      <c r="K17" s="119"/>
+      <c r="L17" s="119"/>
+      <c r="M17" s="119"/>
+      <c r="N17" s="119"/>
+      <c r="O17" s="119"/>
+      <c r="P17" s="119"/>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="115"/>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="117"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -31661,16 +31673,16 @@
       <c r="G18" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="117"/>
-      <c r="P18" s="117"/>
+      <c r="I18" s="119"/>
+      <c r="J18" s="119"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="119"/>
+      <c r="M18" s="119"/>
+      <c r="N18" s="119"/>
+      <c r="O18" s="119"/>
+      <c r="P18" s="119"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -31687,22 +31699,22 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="56" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -31710,7 +31722,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="57" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
inplementing ssOS to Droidbot
</commit_message>
<xml_diff>
--- a/documentation/Droidbot.xlsx
+++ b/documentation/Droidbot.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="930" activeTab="2"/>
@@ -33,12 +33,12 @@
     <definedName name="V_in" localSheetId="5">'Light sensor #2'!$B$5</definedName>
     <definedName name="V_in">'Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="323">
   <si>
     <t>PF0 (SW 2)</t>
   </si>
@@ -1327,15 +1327,30 @@
   <si>
     <t>Pull up, low level interrupt</t>
   </si>
+  <si>
+    <t>U1Rx PB0 is RxD</t>
+  </si>
+  <si>
+    <t>U1Tx PB1 is TxD</t>
+  </si>
+  <si>
+    <t>UART RX</t>
+  </si>
+  <si>
+    <t>UART TX</t>
+  </si>
+  <si>
+    <t>reserved for CC2650</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1941,7 +1956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2122,6 +2137,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2164,7 +2180,7 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2798,7 +2814,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2818,7 +2834,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -7094,7 +7110,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7126,10 +7142,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7161,7 +7176,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7337,14 +7351,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" bestFit="1" customWidth="1"/>
@@ -7352,7 +7366,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19.5" customHeight="1">
       <c r="A1" s="61"/>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -7370,7 +7384,7 @@
       <c r="O1" s="61"/>
       <c r="P1" s="61"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="61"/>
       <c r="B2" s="60" t="s">
         <v>160</v>
@@ -7394,10 +7408,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="61"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="61" t="s">
         <v>194</v>
       </c>
@@ -7408,7 +7422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="61" t="s">
         <v>194</v>
       </c>
@@ -7422,7 +7436,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" s="61"/>
       <c r="B6" s="1" t="s">
         <v>157</v>
@@ -7431,7 +7445,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" s="61"/>
       <c r="B7" s="1" t="s">
         <v>157</v>
@@ -7440,7 +7454,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="61"/>
       <c r="B8" s="1" t="s">
         <v>157</v>
@@ -7449,10 +7463,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="61"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="61"/>
       <c r="B10" s="1" t="s">
         <v>144</v>
@@ -7461,7 +7475,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="61"/>
       <c r="B11" s="1" t="s">
         <v>144</v>
@@ -7470,7 +7484,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="61" t="s">
         <v>195</v>
       </c>
@@ -7481,7 +7495,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="61" t="s">
         <v>195</v>
       </c>
@@ -7492,7 +7506,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="61" t="s">
         <v>195</v>
       </c>
@@ -7503,7 +7517,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="61" t="s">
         <v>195</v>
       </c>
@@ -7514,7 +7528,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="61"/>
       <c r="B16" s="1" t="s">
         <v>144</v>
@@ -7523,7 +7537,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="61"/>
       <c r="B17" s="1" t="s">
         <v>144</v>
@@ -7532,7 +7546,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="61" t="s">
         <v>195</v>
       </c>
@@ -7543,7 +7557,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="61"/>
       <c r="B19" s="1" t="s">
         <v>147</v>
@@ -7552,10 +7566,10 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="61"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="61" t="s">
         <v>195</v>
       </c>
@@ -7566,7 +7580,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="61"/>
       <c r="B22" s="1" t="s">
         <v>154</v>
@@ -7575,7 +7589,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="61"/>
       <c r="B23" s="46" t="s">
         <v>154</v>
@@ -7584,47 +7598,47 @@
         <v>173</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="61"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="61"/>
       <c r="B25" s="86"/>
       <c r="C25" s="86" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="61"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="61"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="61"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="61"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="61"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="61"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="61"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="61"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="61"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="61"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="61"/>
     </row>
   </sheetData>
@@ -7634,14 +7648,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="F2:M2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="13" width="8.140625" customWidth="1"/>
     <col min="258" max="269" width="8.140625" customWidth="1"/>
@@ -7709,7 +7723,7 @@
     <col min="16130" max="16141" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1">
       <c r="A1" s="17">
         <v>0</v>
       </c>
@@ -7748,7 +7762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="48" customHeight="1" thickTop="1">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -7785,7 +7799,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="48" customHeight="1">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -7822,7 +7836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="48" customHeight="1">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -7849,7 +7863,7 @@
       <c r="L4" s="20"/>
       <c r="M4" s="22"/>
     </row>
-    <row r="5" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="48" customHeight="1">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -7873,7 +7887,7 @@
       <c r="L5" s="20"/>
       <c r="M5" s="22"/>
     </row>
-    <row r="6" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="48" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="20" t="s">
         <v>64</v>
@@ -7895,7 +7909,7 @@
       <c r="L6" s="20"/>
       <c r="M6" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="48" customHeight="1" thickBot="1">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -7930,21 +7944,21 @@
       <c r="L7" s="24"/>
       <c r="M7" s="25"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" ht="15.75" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CH55"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="BM17" sqref="BM17:BO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="257" max="340" width="2.85546875" customWidth="1"/>
@@ -8012,7 +8026,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:86" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -8101,7 +8115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:86" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8191,7 +8205,7 @@
         <v>const char Name_goes_here[] = {</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:86" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -8281,7 +8295,7 @@
         <v xml:space="preserve">  0x08, 0x08, 0x08, 0x08, 0x08, 0x18, 0x18, 0x18, 0x38, 0x30, 0x30, 0x30, 0x70, 0xF0,</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:86" ht="16.5" customHeight="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -8405,7 +8419,7 @@
         <v xml:space="preserve">  0xE0, 0xC0, 0xC0, 0x80, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:86" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -8531,7 +8545,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:86" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -8649,7 +8663,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:86" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -8763,7 +8777,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x80, 0xC0, 0xC0, 0xE0, 0xE0, 0xF0, 0x70,</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:86" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -8875,7 +8889,7 @@
         <v xml:space="preserve">  0x70, 0x30, 0x30, 0x18, 0x18, 0x18, 0x18, 0x08, 0x08, 0x08, 0x08, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:86" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -8989,7 +9003,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:86" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -9101,7 +9115,7 @@
         <v xml:space="preserve">  0x01, 0x03, 0x03, 0x03, 0x07, 0x0F, 0x0E, 0x0C, 0x1C, 0x38, 0x38, 0xB8, 0xF8, 0xF0,</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:86" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -9215,7 +9229,7 @@
         <v xml:space="preserve">  0xF0, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xFC, 0xFC, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8,</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:86" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -9375,7 +9389,7 @@
         <v xml:space="preserve">  0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF8, 0xF0, 0xE0, 0xE0, 0xF0, 0xF0, 0xF0,</v>
       </c>
     </row>
-    <row r="13" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:86" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -9541,7 +9555,7 @@
         <v xml:space="preserve">  0xF0, 0x78, 0x38, 0x3C, 0x1C, 0x1F, 0x0F, 0x07, 0x03, 0x03, 0x01, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="14" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:86" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -9705,7 +9719,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="15" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:86" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -9859,7 +9873,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="16" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:86" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -10013,7 +10027,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x06, 0x0F, 0x0F, 0x0F, 0x0F,</v>
       </c>
     </row>
-    <row r="17" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:86" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -10177,7 +10191,7 @@
         <v xml:space="preserve">  0x0F, 0x07, 0x07, 0x07, 0x1F, 0xFF, 0xFF, 0xCF, 0xC7, 0xE7, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="18" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:86" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -10345,7 +10359,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xE7, 0xC7, 0xCF, 0xFF, 0xFF, 0x1F, 0x0F, 0x1F, 0x1F, 0x1F, 0x1F,</v>
       </c>
     </row>
-    <row r="19" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:86" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -10515,7 +10529,7 @@
         <v xml:space="preserve">  0x1F, 0x1F, 0x1E, 0x0E, 0x04, 0x00, 0x00, 0x00, 0x0F, 0x05, 0x0B, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="20" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:86" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -10667,7 +10681,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="21" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:86" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -10797,7 +10811,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="22" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:86" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -10913,7 +10927,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="23" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:86" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -11037,7 +11051,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x01, 0x07, 0x1F, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="24" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:86" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -11161,7 +11175,7 @@
         <v xml:space="preserve">  0xFF, 0xFF, 0xFF, 0xFF, 0x1F, 0x07, 0x03, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="25" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:86" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -11283,7 +11297,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="26" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:86" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -11403,7 +11417,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="27" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:86" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -11521,7 +11535,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="28" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:86" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -11635,7 +11649,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="29" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:86" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -11749,7 +11763,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x3C, 0x7F, 0x7F, 0xEF, 0xDF, 0xFF, 0xFF,</v>
       </c>
     </row>
-    <row r="30" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:86" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -11859,7 +11873,7 @@
         <v xml:space="preserve">  0xDF, 0xEF, 0x7F, 0x3F, 0x38, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="31" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:86" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -11969,7 +11983,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="32" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:86" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -12079,7 +12093,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="33" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:86" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -12189,7 +12203,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="34" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:86" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -12299,7 +12313,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="35" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:86" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -12411,7 +12425,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="36" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:86" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -12525,7 +12539,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="37" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:86" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -12635,7 +12649,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00,</v>
       </c>
     </row>
-    <row r="38" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:86" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -12745,7 +12759,7 @@
         <v xml:space="preserve">  0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00, 0x00</v>
       </c>
     </row>
-    <row r="39" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:86" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -12852,7 +12866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -12950,7 +12964,7 @@
       <c r="CE40" s="11"/>
       <c r="CF40" s="12"/>
     </row>
-    <row r="41" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -13039,7 +13053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:86" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -13128,7 +13142,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:86" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -13217,7 +13231,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:86" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -13303,7 +13317,7 @@
       <c r="CE44" s="11"/>
       <c r="CF44" s="12"/>
     </row>
-    <row r="45" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:86" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -13389,7 +13403,7 @@
       <c r="CE45" s="11"/>
       <c r="CF45" s="12"/>
     </row>
-    <row r="46" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:86" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -13475,7 +13489,7 @@
       <c r="CE46" s="11"/>
       <c r="CF46" s="12"/>
     </row>
-    <row r="47" spans="1:86" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:86" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -13561,7 +13575,7 @@
       <c r="CE47" s="11"/>
       <c r="CF47" s="12"/>
     </row>
-    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:86" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -13647,7 +13661,7 @@
       <c r="CE48" s="15"/>
       <c r="CF48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>08</v>
@@ -13985,7 +13999,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -14323,7 +14337,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -14661,7 +14675,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -14999,7 +15013,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -15337,7 +15351,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -15687,14 +15701,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GB55"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="CQ36" sqref="CQ36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="84" width="2.85546875" customWidth="1"/>
     <col min="101" max="188" width="3.42578125" customWidth="1"/>
@@ -15763,7 +15777,7 @@
     <col min="16129" max="16212" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:184" ht="16.5" customHeight="1">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -15936,7 +15950,7 @@
       <c r="GA1" s="7"/>
       <c r="GB1" s="8"/>
     </row>
-    <row r="2" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:184" ht="16.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -16110,7 +16124,7 @@
       <c r="GA2" s="11"/>
       <c r="GB2" s="12"/>
     </row>
-    <row r="3" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:184" ht="16.5" customHeight="1">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -16340,7 +16354,7 @@
       <c r="GA3" s="11"/>
       <c r="GB3" s="12"/>
     </row>
-    <row r="4" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:184" ht="16.5" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -16542,7 +16556,7 @@
       <c r="GA4" s="11"/>
       <c r="GB4" s="12"/>
     </row>
-    <row r="5" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:184" ht="16.5" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -16744,7 +16758,7 @@
       <c r="GA5" s="11"/>
       <c r="GB5" s="12"/>
     </row>
-    <row r="6" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:184" ht="16.5" customHeight="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -16958,7 +16972,7 @@
       <c r="GA6" s="11"/>
       <c r="GB6" s="12"/>
     </row>
-    <row r="7" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:184" ht="16.5" customHeight="1">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -17174,7 +17188,7 @@
       <c r="GA7" s="11"/>
       <c r="GB7" s="12"/>
     </row>
-    <row r="8" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:184" ht="16.5" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -17386,7 +17400,7 @@
       <c r="GA8" s="11"/>
       <c r="GB8" s="12"/>
     </row>
-    <row r="9" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:184" ht="16.5" customHeight="1">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
@@ -17598,7 +17612,7 @@
       <c r="GA9" s="11"/>
       <c r="GB9" s="12"/>
     </row>
-    <row r="10" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:184" ht="16.5" customHeight="1">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -17824,7 +17838,7 @@
       <c r="GA10" s="11"/>
       <c r="GB10" s="12"/>
     </row>
-    <row r="11" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:184" ht="16.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -17998,7 +18012,7 @@
       <c r="GA11" s="11"/>
       <c r="GB11" s="12"/>
     </row>
-    <row r="12" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:184" ht="16.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -18184,7 +18198,7 @@
       <c r="GA12" s="11"/>
       <c r="GB12" s="12"/>
     </row>
-    <row r="13" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:184" ht="16.5" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -18382,7 +18396,7 @@
       <c r="GA13" s="11"/>
       <c r="GB13" s="12"/>
     </row>
-    <row r="14" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:184" ht="16.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -18576,7 +18590,7 @@
       <c r="GA14" s="11"/>
       <c r="GB14" s="12"/>
     </row>
-    <row r="15" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:184" ht="16.5" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -18762,7 +18776,7 @@
       <c r="GA15" s="11"/>
       <c r="GB15" s="12"/>
     </row>
-    <row r="16" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:184" ht="16.5" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -18954,7 +18968,7 @@
       <c r="GA16" s="11"/>
       <c r="GB16" s="12"/>
     </row>
-    <row r="17" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:184" ht="16.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -19148,7 +19162,7 @@
       <c r="GA17" s="11"/>
       <c r="GB17" s="12"/>
     </row>
-    <row r="18" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:184" ht="16.5" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -19342,7 +19356,7 @@
       <c r="GA18" s="11"/>
       <c r="GB18" s="12"/>
     </row>
-    <row r="19" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:184" ht="16.5" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -19524,7 +19538,7 @@
       <c r="GA19" s="11"/>
       <c r="GB19" s="12"/>
     </row>
-    <row r="20" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:184" ht="16.5" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -19706,7 +19720,7 @@
       <c r="GA20" s="11"/>
       <c r="GB20" s="12"/>
     </row>
-    <row r="21" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:184" ht="16.5" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -19900,7 +19914,7 @@
       <c r="GA21" s="11"/>
       <c r="GB21" s="12"/>
     </row>
-    <row r="22" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:184" ht="16.5" customHeight="1">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -20088,7 +20102,7 @@
       <c r="GA22" s="11"/>
       <c r="GB22" s="12"/>
     </row>
-    <row r="23" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:184" ht="16.5" customHeight="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -20282,7 +20296,7 @@
       <c r="GA23" s="11"/>
       <c r="GB23" s="12"/>
     </row>
-    <row r="24" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:184" ht="16.5" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -20464,7 +20478,7 @@
       <c r="GA24" s="11"/>
       <c r="GB24" s="12"/>
     </row>
-    <row r="25" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:184" ht="16.5" customHeight="1">
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -20648,7 +20662,7 @@
       <c r="GA25" s="11"/>
       <c r="GB25" s="12"/>
     </row>
-    <row r="26" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:184" ht="16.5" customHeight="1">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -20874,7 +20888,7 @@
       <c r="GA26" s="11"/>
       <c r="GB26" s="12"/>
     </row>
-    <row r="27" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:184" ht="16.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -21056,7 +21070,7 @@
       <c r="GA27" s="11"/>
       <c r="GB27" s="12"/>
     </row>
-    <row r="28" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:184" ht="16.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -21238,7 +21252,7 @@
       <c r="GA28" s="11"/>
       <c r="GB28" s="12"/>
     </row>
-    <row r="29" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:184" ht="16.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -21438,7 +21452,7 @@
       <c r="GA29" s="11"/>
       <c r="GB29" s="12"/>
     </row>
-    <row r="30" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:184" ht="16.5" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -21656,7 +21670,7 @@
       <c r="GA30" s="11"/>
       <c r="GB30" s="12"/>
     </row>
-    <row r="31" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:184" ht="16.5" customHeight="1">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -21844,7 +21858,7 @@
       <c r="GA31" s="11"/>
       <c r="GB31" s="12"/>
     </row>
-    <row r="32" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:184" ht="16.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -22036,7 +22050,7 @@
       <c r="GA32" s="11"/>
       <c r="GB32" s="12"/>
     </row>
-    <row r="33" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:184" ht="16.5" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -22228,7 +22242,7 @@
       <c r="GA33" s="11"/>
       <c r="GB33" s="12"/>
     </row>
-    <row r="34" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:184" ht="16.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -22418,7 +22432,7 @@
       <c r="GA34" s="11"/>
       <c r="GB34" s="12"/>
     </row>
-    <row r="35" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:184" ht="16.5" customHeight="1">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -22608,7 +22622,7 @@
       <c r="GA35" s="11"/>
       <c r="GB35" s="12"/>
     </row>
-    <row r="36" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:184" ht="16.5" customHeight="1">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -22800,7 +22814,7 @@
       <c r="GA36" s="11"/>
       <c r="GB36" s="12"/>
     </row>
-    <row r="37" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:184" ht="16.5" customHeight="1">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -22992,7 +23006,7 @@
       <c r="GA37" s="11"/>
       <c r="GB37" s="12"/>
     </row>
-    <row r="38" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:184" ht="16.5" customHeight="1">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -23184,7 +23198,7 @@
       <c r="GA38" s="11"/>
       <c r="GB38" s="12"/>
     </row>
-    <row r="39" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:184" ht="16.5" customHeight="1">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -23377,7 +23391,7 @@
       <c r="GA39" s="11"/>
       <c r="GB39" s="12"/>
     </row>
-    <row r="40" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:184" ht="16.5" customHeight="1">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -23601,7 +23615,7 @@
       <c r="GA40" s="11"/>
       <c r="GB40" s="12"/>
     </row>
-    <row r="41" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:184" ht="16.5" customHeight="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -23796,7 +23810,7 @@
       <c r="GA41" s="11"/>
       <c r="GB41" s="12"/>
     </row>
-    <row r="42" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:184" ht="16.5" customHeight="1">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -24029,7 +24043,7 @@
       <c r="GA42" s="11"/>
       <c r="GB42" s="12"/>
     </row>
-    <row r="43" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:184" ht="16.5" customHeight="1">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -24252,7 +24266,7 @@
       <c r="GA43" s="11"/>
       <c r="GB43" s="12"/>
     </row>
-    <row r="44" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:184" ht="16.5" customHeight="1">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -24454,7 +24468,7 @@
       <c r="GA44" s="11"/>
       <c r="GB44" s="12"/>
     </row>
-    <row r="45" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:184" ht="16.5" customHeight="1">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -24736,7 +24750,7 @@
       <c r="GA45" s="11"/>
       <c r="GB45" s="12"/>
     </row>
-    <row r="46" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:184" ht="16.5" customHeight="1">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -24914,7 +24928,7 @@
       <c r="GA46" s="11"/>
       <c r="GB46" s="12"/>
     </row>
-    <row r="47" spans="1:184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:184" ht="16.5" customHeight="1">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -25116,7 +25130,7 @@
       <c r="GA47" s="11"/>
       <c r="GB47" s="12"/>
     </row>
-    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:184" ht="16.5" customHeight="1" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -25288,7 +25302,7 @@
       <c r="GA48" s="15"/>
       <c r="GB48" s="16"/>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:84">
       <c r="A50" t="str">
         <f>DEC2HEX(128*(A8&gt;0)+64*(A7&gt;0)+32*(A6&gt;0)+16*(A5&gt;0)+8*(A4&gt;0)+4*(A3&gt;0)+2*(A2&gt;0)+1*(A1&gt;0),2)</f>
         <v>00</v>
@@ -25626,7 +25640,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:84">
       <c r="A51" t="str">
         <f>DEC2HEX(128*(A16&gt;0)+64*(A15&gt;0)+32*(A14&gt;0)+16*(A13&gt;0)+8*(A12&gt;0)+4*(A11&gt;0)+2*(A10&gt;0)+1*(A9&gt;0),2)</f>
         <v>00</v>
@@ -25964,7 +25978,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:84">
       <c r="A52" t="str">
         <f>DEC2HEX(128*(A24&gt;0)+64*(A23&gt;0)+32*(A22&gt;0)+16*(A21&gt;0)+8*(A20&gt;0)+4*(A19&gt;0)+2*(A18&gt;0)+1*(A17&gt;0),2)</f>
         <v>00</v>
@@ -26302,7 +26316,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:84">
       <c r="A53" t="str">
         <f>DEC2HEX(128*(A32&gt;0)+64*(A31&gt;0)+32*(A30&gt;0)+16*(A29&gt;0)+8*(A28&gt;0)+4*(A27&gt;0)+2*(A26&gt;0)+1*(A25&gt;0),2)</f>
         <v>00</v>
@@ -26640,7 +26654,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:84">
       <c r="A54" t="str">
         <f>DEC2HEX(128*(A40&gt;0)+64*(A39&gt;0)+32*(A38&gt;0)+16*(A37&gt;0)+8*(A36&gt;0)+4*(A35&gt;0)+2*(A34&gt;0)+1*(A33&gt;0),2)</f>
         <v>00</v>
@@ -26978,7 +26992,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:84">
       <c r="A55" t="str">
         <f>DEC2HEX(128*(A48&gt;0)+64*(A47&gt;0)+32*(A46&gt;0)+16*(A45&gt;0)+8*(A44&gt;0)+4*(A43&gt;0)+2*(A42&gt;0)+1*(A41&gt;0),2)</f>
         <v>00</v>
@@ -27623,14 +27637,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="AY48" sqref="AY48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="62" customWidth="1"/>
     <col min="2" max="7" width="3.7109375" style="62" customWidth="1"/>
@@ -27646,7 +27660,7 @@
     <col min="40" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39">
       <c r="A1" s="64"/>
       <c r="B1" s="64"/>
       <c r="C1" s="65"/>
@@ -27683,7 +27697,7 @@
       <c r="AL1" s="65"/>
       <c r="AM1" s="65"/>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39">
       <c r="A2" s="64"/>
       <c r="B2" s="66"/>
       <c r="C2" s="66">
@@ -27732,7 +27746,7 @@
       <c r="AL2" s="66"/>
       <c r="AM2" s="65"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39">
       <c r="A3" s="64"/>
       <c r="B3" s="66">
         <v>1</v>
@@ -27791,7 +27805,7 @@
       <c r="AL3" s="66"/>
       <c r="AM3" s="65"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39">
       <c r="A4" s="64"/>
       <c r="B4" s="66"/>
       <c r="C4" s="66">
@@ -27852,7 +27866,7 @@
       <c r="AL4" s="66"/>
       <c r="AM4" s="65"/>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39">
       <c r="A5" s="64"/>
       <c r="B5" s="66">
         <v>1</v>
@@ -27917,7 +27931,7 @@
       </c>
       <c r="AM5" s="65"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39">
       <c r="A6" s="64"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66">
@@ -27982,7 +27996,7 @@
       </c>
       <c r="AM6" s="65"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39">
       <c r="A7" s="64"/>
       <c r="B7" s="66">
         <v>1</v>
@@ -28049,7 +28063,7 @@
       <c r="AL7" s="66"/>
       <c r="AM7" s="65"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39">
       <c r="A8" s="64"/>
       <c r="B8" s="66"/>
       <c r="C8" s="66">
@@ -28110,7 +28124,7 @@
       <c r="AL8" s="66"/>
       <c r="AM8" s="64"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39">
       <c r="A9" s="64"/>
       <c r="B9" s="66">
         <v>1</v>
@@ -28171,7 +28185,7 @@
       <c r="AL9" s="66"/>
       <c r="AM9" s="64"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39">
       <c r="A10" s="64"/>
       <c r="B10" s="64"/>
       <c r="C10" s="64"/>
@@ -28208,7 +28222,7 @@
       <c r="AL10" s="64"/>
       <c r="AM10" s="64"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39">
       <c r="B12" s="63" t="str">
         <f>DEC2HEX(128*(B9&gt;0)+64*(B8&gt;0)+32*(B7&gt;0)+16*(B6&gt;0)+8*(B5&gt;0)+4*(B4&gt;0)+2*(B3&gt;0)+1*(B2&gt;0),2)</f>
         <v>AA</v>
@@ -28310,7 +28324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39">
       <c r="A14" s="64"/>
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
@@ -28347,7 +28361,7 @@
       <c r="AL14" s="65"/>
       <c r="AM14" s="65"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39">
       <c r="A15" s="64"/>
       <c r="B15" s="66"/>
       <c r="C15" s="66"/>
@@ -28390,7 +28404,7 @@
       <c r="AL15" s="66"/>
       <c r="AM15" s="65"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39">
       <c r="A16" s="64"/>
       <c r="B16" s="66"/>
       <c r="C16" s="66"/>
@@ -28443,7 +28457,7 @@
       <c r="AL16" s="66"/>
       <c r="AM16" s="65"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39">
       <c r="A17" s="64"/>
       <c r="B17" s="66">
         <v>1</v>
@@ -28516,7 +28530,7 @@
       </c>
       <c r="AM17" s="65"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39">
       <c r="A18" s="64"/>
       <c r="B18" s="66"/>
       <c r="C18" s="66">
@@ -28579,7 +28593,7 @@
       </c>
       <c r="AM18" s="65"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39">
       <c r="A19" s="64"/>
       <c r="B19" s="66"/>
       <c r="C19" s="66"/>
@@ -28630,7 +28644,7 @@
       </c>
       <c r="AM19" s="65"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39">
       <c r="A20" s="64"/>
       <c r="B20" s="66"/>
       <c r="C20" s="66"/>
@@ -28683,7 +28697,7 @@
       </c>
       <c r="AM20" s="65"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39">
       <c r="A21" s="64"/>
       <c r="B21" s="66"/>
       <c r="C21" s="66">
@@ -28742,7 +28756,7 @@
       <c r="AL21" s="66"/>
       <c r="AM21" s="64"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39">
       <c r="A22" s="64"/>
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
@@ -28785,7 +28799,7 @@
       <c r="AL22" s="66"/>
       <c r="AM22" s="64"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39">
       <c r="A23" s="64"/>
       <c r="B23" s="64"/>
       <c r="C23" s="64"/>
@@ -28822,7 +28836,7 @@
       <c r="AL23" s="64"/>
       <c r="AM23" s="64"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39">
       <c r="B25" s="63" t="str">
         <f>DEC2HEX(128*(B22&gt;0)+64*(B21&gt;0)+32*(B20&gt;0)+16*(B19&gt;0)+8*(B18&gt;0)+4*(B17&gt;0)+2*(B16&gt;0)+1*(B15&gt;0),2)</f>
         <v>04</v>
@@ -29010,21 +29024,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="68" t="s">
         <v>166</v>
       </c>
@@ -29032,7 +29046,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -29046,7 +29060,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -29060,7 +29074,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="L4">
         <v>1</v>
       </c>
@@ -29071,7 +29085,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="68" t="s">
         <v>167</v>
       </c>
@@ -29085,7 +29099,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="L6">
         <v>2</v>
       </c>
@@ -29096,7 +29110,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="L7">
         <v>3</v>
       </c>
@@ -29107,22 +29121,22 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="L8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="L9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="L10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="L11">
         <v>7</v>
       </c>
@@ -29140,14 +29154,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -29158,7 +29172,7 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -29181,34 +29195,34 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+    <row r="2" spans="1:8" ht="15" customHeight="1">
+      <c r="A2" s="108" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="107"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="108"/>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="107"/>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="108"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -29229,8 +29243,8 @@
       </c>
       <c r="H4" s="72"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107"/>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="108"/>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -29251,8 +29265,8 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="A6" s="108"/>
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
@@ -29265,8 +29279,8 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="108"/>
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
@@ -29287,8 +29301,8 @@
       </c>
       <c r="H7" s="59"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
+    <row r="8" spans="1:8">
+      <c r="A8" s="108"/>
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
@@ -29309,8 +29323,8 @@
       </c>
       <c r="H8" s="58"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="108"/>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
@@ -29331,34 +29345,46 @@
       </c>
       <c r="H9" s="101"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="107" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="108" t="s">
         <v>276</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
+    <row r="12" spans="1:8">
+      <c r="A12" s="108"/>
       <c r="B12" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="108"/>
       <c r="B13" s="1" t="s">
         <v>279</v>
       </c>
@@ -29379,8 +29405,8 @@
       </c>
       <c r="H13" s="104"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
+    <row r="14" spans="1:8">
+      <c r="A14" s="108"/>
       <c r="B14" s="1" t="s">
         <v>280</v>
       </c>
@@ -29401,8 +29427,8 @@
       </c>
       <c r="H14" s="105"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+    <row r="15" spans="1:8">
+      <c r="A15" s="108"/>
       <c r="B15" s="1" t="s">
         <v>281</v>
       </c>
@@ -29413,8 +29439,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+    <row r="16" spans="1:8">
+      <c r="A16" s="108"/>
       <c r="B16" s="1" t="s">
         <v>282</v>
       </c>
@@ -29425,8 +29451,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+    <row r="17" spans="1:8">
+      <c r="A17" s="108"/>
       <c r="B17" s="1" t="s">
         <v>283</v>
       </c>
@@ -29437,52 +29463,52 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="107" t="s">
+    <row r="19" spans="1:8">
+      <c r="A19" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="106"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
+      <c r="C19" s="107"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="107"/>
-      <c r="B20" s="106"/>
-      <c r="C20" s="106"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="106"/>
+    <row r="20" spans="1:8">
+      <c r="A20" s="108"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="107"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
-      <c r="B21" s="106"/>
-      <c r="C21" s="106"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
+    <row r="21" spans="1:8">
+      <c r="A21" s="108"/>
+      <c r="B21" s="107"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
-      <c r="B22" s="106"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="106"/>
+    <row r="22" spans="1:8">
+      <c r="A22" s="108"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="107"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="107"/>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="108"/>
       <c r="B23" s="99" t="s">
         <v>208</v>
       </c>
@@ -29497,8 +29523,8 @@
       <c r="G23" s="99"/>
       <c r="H23" s="99"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="107"/>
+    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="A24" s="108"/>
       <c r="B24" s="99" t="s">
         <v>209</v>
       </c>
@@ -29515,8 +29541,8 @@
       <c r="G24" s="99"/>
       <c r="H24" s="99"/>
     </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="107"/>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="A25" s="108"/>
       <c r="B25" s="99" t="s">
         <v>28</v>
       </c>
@@ -29533,8 +29559,8 @@
       <c r="G25" s="99"/>
       <c r="H25" s="99"/>
     </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
+    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="A26" s="108"/>
       <c r="B26" s="99" t="s">
         <v>29</v>
       </c>
@@ -29553,8 +29579,8 @@
       <c r="G26" s="99"/>
       <c r="H26" s="99"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="107" t="s">
+    <row r="28" spans="1:8">
+      <c r="A28" s="108" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="102" t="s">
@@ -29575,8 +29601,8 @@
       </c>
       <c r="H28" s="102"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
+    <row r="29" spans="1:8">
+      <c r="A29" s="108"/>
       <c r="B29" s="102" t="s">
         <v>22</v>
       </c>
@@ -29595,8 +29621,8 @@
       </c>
       <c r="H29" s="102"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
+    <row r="30" spans="1:8">
+      <c r="A30" s="108"/>
       <c r="B30" s="102" t="s">
         <v>302</v>
       </c>
@@ -29615,8 +29641,8 @@
       </c>
       <c r="H30" s="102"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
+    <row r="31" spans="1:8">
+      <c r="A31" s="108"/>
       <c r="B31" s="102" t="s">
         <v>303</v>
       </c>
@@ -29635,8 +29661,8 @@
       </c>
       <c r="H31" s="102"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
+    <row r="32" spans="1:8">
+      <c r="A32" s="108"/>
       <c r="B32" s="100" t="s">
         <v>268</v>
       </c>
@@ -29657,8 +29683,8 @@
       </c>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
+    <row r="33" spans="1:9">
+      <c r="A33" s="108"/>
       <c r="B33" s="1" t="s">
         <v>253</v>
       </c>
@@ -29679,8 +29705,8 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="107" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" s="108" t="s">
         <v>257</v>
       </c>
       <c r="B35" s="100" t="s">
@@ -29703,8 +29729,8 @@
       </c>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
+    <row r="36" spans="1:9">
+      <c r="A36" s="108"/>
       <c r="B36" s="1" t="s">
         <v>259</v>
       </c>
@@ -29725,8 +29751,8 @@
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
+    <row r="37" spans="1:9">
+      <c r="A37" s="108"/>
       <c r="B37" s="1" t="s">
         <v>260</v>
       </c>
@@ -29747,8 +29773,8 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="107"/>
+    <row r="38" spans="1:9">
+      <c r="A38" s="108"/>
       <c r="B38" s="1" t="s">
         <v>261</v>
       </c>
@@ -29769,8 +29795,8 @@
       </c>
       <c r="H38" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="107" t="s">
+    <row r="40" spans="1:9" ht="15" customHeight="1">
+      <c r="A40" s="108" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -29790,12 +29816,12 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="120" t="s">
+      <c r="I40" s="106" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="107"/>
+    <row r="41" spans="1:9" ht="15" customHeight="1">
+      <c r="A41" s="108"/>
       <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
@@ -29814,8 +29840,8 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="107"/>
+    <row r="42" spans="1:9">
+      <c r="A42" s="108"/>
       <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
@@ -29836,8 +29862,8 @@
       </c>
       <c r="H42" s="98"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="107"/>
+    <row r="43" spans="1:9">
+      <c r="A43" s="108"/>
       <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
@@ -29858,8 +29884,8 @@
       </c>
       <c r="H43" s="72"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="107"/>
+    <row r="44" spans="1:9">
+      <c r="A44" s="108"/>
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
@@ -29877,11 +29903,11 @@
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="120" t="s">
+      <c r="I44" s="106" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="B46" t="s">
         <v>16</v>
       </c>
@@ -29892,7 +29918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="C47" t="s">
         <v>18</v>
       </c>
@@ -29917,56 +29943,56 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P45"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="16:16">
       <c r="P2" s="57" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>316</v>
       </c>
@@ -29981,14 +30007,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -29997,7 +30023,7 @@
     <col min="12" max="13" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -30014,22 +30040,22 @@
       <c r="E1" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="111" t="s">
+      <c r="H1" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="I1" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="115"/>
-      <c r="K1" s="108" t="s">
+      <c r="J1" s="116"/>
+      <c r="K1" s="109" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="113" t="s">
+      <c r="L1" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="M1" s="113"/>
+      <c r="M1" s="114"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -30046,14 +30072,14 @@
       <c r="E2" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="112"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="80" t="s">
         <v>237</v>
       </c>
       <c r="J2" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="80" t="s">
         <v>237</v>
       </c>
@@ -30061,7 +30087,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
         <v>216</v>
       </c>
@@ -30081,20 +30107,20 @@
       <c r="H3" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="I3" s="114" t="s">
+      <c r="I3" s="115" t="s">
         <v>229</v>
       </c>
-      <c r="J3" s="115"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="114" t="s">
+      <c r="J3" s="116"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="M3" s="115"/>
+      <c r="M3" s="116"/>
       <c r="P3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>217</v>
       </c>
@@ -30135,7 +30161,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="18">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -30168,7 +30194,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -30195,7 +30221,7 @@
       </c>
       <c r="Q6" s="85"/>
     </row>
-    <row r="7" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="18">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -30231,7 +30257,7 @@
       </c>
       <c r="Q7" s="86"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -30253,7 +30279,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -30284,7 +30310,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -30315,7 +30341,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -30358,14 +30384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" hidden="1" customWidth="1"/>
@@ -30374,7 +30400,7 @@
     <col min="12" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -30391,26 +30417,26 @@
       <c r="E1" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="111" t="s">
+      <c r="H1" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="I1" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="115"/>
-      <c r="K1" s="108" t="s">
+      <c r="J1" s="116"/>
+      <c r="K1" s="109" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="113" t="s">
+      <c r="L1" s="114" t="s">
         <v>251</v>
       </c>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113" t="s">
+      <c r="M1" s="114"/>
+      <c r="N1" s="114" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="113"/>
+      <c r="O1" s="114"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>215</v>
       </c>
@@ -30427,14 +30453,14 @@
       <c r="E2" s="77" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="112"/>
+      <c r="H2" s="113"/>
       <c r="I2" s="80" t="s">
         <v>237</v>
       </c>
       <c r="J2" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="109"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="80" t="s">
         <v>244</v>
       </c>
@@ -30448,7 +30474,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>247</v>
       </c>
@@ -30468,22 +30494,22 @@
       <c r="H3" s="80" t="s">
         <v>227</v>
       </c>
-      <c r="I3" s="114" t="s">
+      <c r="I3" s="115" t="s">
         <v>229</v>
       </c>
-      <c r="J3" s="115"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="114" t="s">
+      <c r="J3" s="116"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="115" t="s">
         <v>219</v>
       </c>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="115"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
+      <c r="O3" s="116"/>
       <c r="T3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>248</v>
       </c>
@@ -30532,7 +30558,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="18">
       <c r="A5" s="1" t="s">
         <v>218</v>
       </c>
@@ -30573,7 +30599,7 @@
         <v>9.6116504854368928E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="H6" s="73">
         <v>10.75</v>
       </c>
@@ -30608,7 +30634,7 @@
       </c>
       <c r="U6" s="85"/>
     </row>
-    <row r="7" spans="1:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="18">
       <c r="A7" s="1" t="s">
         <v>220</v>
       </c>
@@ -30652,7 +30678,7 @@
       </c>
       <c r="U7" s="86"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="H8" s="73">
         <v>107.53</v>
       </c>
@@ -30682,7 +30708,7 @@
         <v>2.9117647058823528</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>222</v>
       </c>
@@ -30721,7 +30747,7 @@
         <v>3.09375</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>224</v>
       </c>
@@ -30760,7 +30786,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="H11" s="73">
         <v>107527</v>
       </c>
@@ -30790,7 +30816,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="L12" s="97" t="s">
         <v>252</v>
       </c>
@@ -30798,7 +30824,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="N13" s="96" t="s">
         <v>252</v>
       </c>
@@ -30828,26 +30854,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A13:A36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>164</v>
       </c>
@@ -30859,14 +30885,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -30878,7 +30904,7 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="36" t="s">
         <v>99</v>
       </c>
@@ -30913,7 +30939,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="36" t="s">
         <v>98</v>
       </c>
@@ -30954,7 +30980,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="36" t="s">
         <v>94</v>
       </c>
@@ -30995,7 +31021,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="36" t="s">
         <v>87</v>
       </c>
@@ -31036,13 +31062,13 @@
       <c r="N4" s="31"/>
       <c r="O4" s="31"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>75.000001875000038</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="30" t="s">
         <v>80</v>
       </c>
@@ -31058,7 +31084,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="30" t="s">
         <v>78</v>
       </c>
@@ -31075,7 +31101,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="D8" t="s">
         <v>170</v>
       </c>
@@ -31083,22 +31109,22 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>7999999</v>
       </c>
@@ -31119,7 +31145,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1599999</v>
       </c>
@@ -31137,7 +31163,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="E20" t="s">
         <v>165</v>
       </c>
@@ -31149,14 +31175,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
@@ -31165,7 +31191,7 @@
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
@@ -31185,7 +31211,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="46" t="s">
         <v>105</v>
       </c>
@@ -31209,7 +31235,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="46" t="s">
         <v>107</v>
       </c>
@@ -31237,15 +31263,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="E4" s="52"/>
       <c r="F4" s="52"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1">
+      <c r="A5" s="118" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="47">
@@ -31266,19 +31292,19 @@
       <c r="G5" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="119" t="s">
+      <c r="I5" s="120" t="s">
         <v>197</v>
       </c>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="119"/>
-      <c r="P5" s="119"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
+    <row r="6" spans="1:16">
+      <c r="A6" s="118"/>
       <c r="B6" s="50">
         <f>B5/60</f>
         <v>0.83333333333333337</v>
@@ -31302,32 +31328,32 @@
       <c r="G6" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="119"/>
-      <c r="P6" s="119"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="120"/>
+      <c r="K6" s="120"/>
+      <c r="L6" s="120"/>
+      <c r="M6" s="120"/>
+      <c r="N6" s="120"/>
+      <c r="O6" s="120"/>
+      <c r="P6" s="120"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
-      <c r="M7" s="119"/>
-      <c r="N7" s="119"/>
-      <c r="O7" s="119"/>
-      <c r="P7" s="119"/>
+      <c r="I7" s="120"/>
+      <c r="J7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="120"/>
+      <c r="N7" s="120"/>
+      <c r="O7" s="120"/>
+      <c r="P7" s="120"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
+    <row r="8" spans="1:16">
+      <c r="A8" s="119" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="50">
@@ -31353,17 +31379,17 @@
       <c r="G8" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="119"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="120"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="118"/>
+    <row r="9" spans="1:16">
+      <c r="A9" s="119"/>
       <c r="B9" s="50">
         <f>B8/10</f>
         <v>10.995574287564278</v>
@@ -31387,17 +31413,17 @@
       <c r="G9" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="119"/>
+      <c r="I9" s="120"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="M9" s="120"/>
+      <c r="N9" s="120"/>
+      <c r="O9" s="120"/>
+      <c r="P9" s="120"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="118"/>
+    <row r="10" spans="1:16">
+      <c r="A10" s="119"/>
       <c r="B10" s="50">
         <f>B8/1000</f>
         <v>0.10995574287564278</v>
@@ -31421,17 +31447,17 @@
       <c r="G10" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="119"/>
-      <c r="J10" s="119"/>
-      <c r="K10" s="119"/>
-      <c r="L10" s="119"/>
-      <c r="M10" s="119"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="119"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="M10" s="120"/>
+      <c r="N10" s="120"/>
+      <c r="O10" s="120"/>
+      <c r="P10" s="120"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="118"/>
+    <row r="11" spans="1:16">
+      <c r="A11" s="119"/>
       <c r="B11" s="50">
         <f>B10*3.6</f>
         <v>0.39584067435231401</v>
@@ -31455,32 +31481,32 @@
       <c r="G11" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="119"/>
-      <c r="P11" s="119"/>
+      <c r="I11" s="120"/>
+      <c r="J11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
+      <c r="P11" s="120"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="119"/>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="119"/>
+      <c r="I12" s="120"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="120"/>
+      <c r="L12" s="120"/>
+      <c r="M12" s="120"/>
+      <c r="N12" s="120"/>
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="117" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="118" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="47">
@@ -31501,17 +31527,17 @@
       <c r="G13" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="I13" s="119"/>
-      <c r="J13" s="119"/>
-      <c r="K13" s="119"/>
-      <c r="L13" s="119"/>
-      <c r="M13" s="119"/>
-      <c r="N13" s="119"/>
-      <c r="O13" s="119"/>
-      <c r="P13" s="119"/>
+      <c r="I13" s="120"/>
+      <c r="J13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="M13" s="120"/>
+      <c r="N13" s="120"/>
+      <c r="O13" s="120"/>
+      <c r="P13" s="120"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+    <row r="14" spans="1:16">
+      <c r="A14" s="118"/>
       <c r="B14" s="50">
         <f>B13*0.007061552</f>
         <v>0.22596966399999999</v>
@@ -31535,17 +31561,17 @@
       <c r="G14" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="119"/>
-      <c r="P14" s="119"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+    <row r="15" spans="1:16">
+      <c r="A15" s="118"/>
       <c r="B15" s="49">
         <f t="shared" ref="B15:E15" si="0">B16</f>
         <v>225.96966399999999</v>
@@ -31569,17 +31595,17 @@
       <c r="G15" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="119"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="119"/>
-      <c r="N15" s="119"/>
-      <c r="O15" s="119"/>
-      <c r="P15" s="119"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="M15" s="120"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="120"/>
+      <c r="P15" s="120"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="117"/>
+    <row r="16" spans="1:16">
+      <c r="A16" s="118"/>
       <c r="B16" s="50">
         <f>B14*1000</f>
         <v>225.96966399999999</v>
@@ -31603,17 +31629,17 @@
       <c r="G16" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="I16" s="119"/>
-      <c r="J16" s="119"/>
-      <c r="K16" s="119"/>
-      <c r="L16" s="119"/>
-      <c r="M16" s="119"/>
-      <c r="N16" s="119"/>
-      <c r="O16" s="119"/>
-      <c r="P16" s="119"/>
+      <c r="I16" s="120"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="120"/>
+      <c r="N16" s="120"/>
+      <c r="O16" s="120"/>
+      <c r="P16" s="120"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="117" t="s">
+    <row r="17" spans="1:16">
+      <c r="A17" s="118" t="s">
         <v>120</v>
       </c>
       <c r="B17" s="50">
@@ -31639,17 +31665,17 @@
       <c r="G17" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119"/>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="119"/>
-      <c r="N17" s="119"/>
-      <c r="O17" s="119"/>
-      <c r="P17" s="119"/>
+      <c r="I17" s="120"/>
+      <c r="J17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="M17" s="120"/>
+      <c r="N17" s="120"/>
+      <c r="O17" s="120"/>
+      <c r="P17" s="120"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="117"/>
+    <row r="18" spans="1:16">
+      <c r="A18" s="118"/>
       <c r="B18" s="50">
         <f>B17/9.81</f>
         <v>1.0968868695694383</v>
@@ -31673,16 +31699,16 @@
       <c r="G18" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="I18" s="119"/>
-      <c r="J18" s="119"/>
-      <c r="K18" s="119"/>
-      <c r="L18" s="119"/>
-      <c r="M18" s="119"/>
-      <c r="N18" s="119"/>
-      <c r="O18" s="119"/>
-      <c r="P18" s="119"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="M18" s="120"/>
+      <c r="N18" s="120"/>
+      <c r="O18" s="120"/>
+      <c r="P18" s="120"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="B19" t="s">
         <v>123</v>
       </c>
@@ -31699,22 +31725,22 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="54" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="55" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="56" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>132</v>
       </c>
@@ -31722,7 +31748,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="B25" s="57" t="s">
         <v>131</v>
       </c>

</xml_diff>